<commit_message>
commit before update (minor)
</commit_message>
<xml_diff>
--- a/Blik/Interventiebeleid tabak.xlsx
+++ b/Blik/Interventiebeleid tabak.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="12" windowWidth="15180" windowHeight="8580"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="15180" windowHeight="8520"/>
   </bookViews>
   <sheets>
     <sheet name="Specifiek" sheetId="1" r:id="rId1"/>
@@ -13,48 +13,15 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Specifiek!$A$1:$R$45</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="223">
-  <si>
-    <t xml:space="preserve">Door de Staat of ander openbaar lichaam beheerde gebouwen of inrichtingen;                             gebouwen of inrichtingen voor de gezondheidszorg, welzijn, maatschappelijke dienstverlening, kunst en cultuur, sport, sociaal-cultureel werk of onderwijs;                  overdekt winkelcentrum;
-evenementenhal;
-congrescentrum;
-luchthaven; 
-ruimte bestemd voor passagiers die gebruik maken van middelen voor personenvervoer. 
-ruimte, gebouw of inrichting waar een werknemer zijn werkzaamheden verricht/pleegt te verrichten; horeca-inrichtingen;      middelen van personenvervoer; vliegtuigen tijdens gebruik voor burgerluchtvaart op vluchten van en naar op Nederlands grondgebied gelegen luchthavens.    </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="228">
   <si>
     <t>10.1 a;    10.1 b;     10.1 c;     10.1 d;    10.1 e;     10.1 f;     10.1 g.</t>
   </si>
   <si>
-    <t xml:space="preserve">Door de Staat of ander openbaar lichaam beheerde gebouwen of inrichtingen;                            gebouwen of inrichtingen voor de gezondheidszorg, welzijn, maatschappelijke dienstverlening, kunst en cultuur, sport, sociaal-cultureel werk of onderwijs;                overdekt winkelcentrum;
-evenementenhal;
-congrescentrum;
-luchthaven; 
-ruimte bestemd voor passagiers die gebruik maken van middelen voor personenvervoer. 
-ruimte, gebouw of inrichting waar een werknemer zijn werkzaamheden verricht/pleegt te verrichten;                                               horeca-inrichtingen; middelen van personenvervoer; vliegtuigen tijdens gebruik voor burgerluchtvaart op vluchten van en naar op Nederlands grondgebied gelegen luchthavens.    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Door de Staat of ander openbaar lichaam beheerde gebouwen of inrichtingen;                            gebouwen of inrichtingen voor de gezondheidszorg, welzijn, maatschappelijke dienstverlening, kunst en cultuur, sport, sociaal-cultureel werk of onderwijs;                 overdekt winkelcentrum;
-evenementenhal;
-congrescentrum;
-luchthaven; 
-ruimte bestemd voor passagiers die gebruik maken van middelen voor personenvervoer. 
-ruimte,                                             gebouw of inrichting waar een werknemer zijn werkzaamheden verricht/pleegt te verrichten;                horeca-inrichtingen;                middelen van personenvervoer;   vliegtuigen tijdens gebruik voor burgerluchtvaart op vluchten van en naar op Nederlands grondgebied gelegen luchthavens.    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Door de Staat of ander openbaar lichaam beheerde gebouwen of inrichtingen;                             gebouwen of inrichtingen voor de gezondheidszorg, welzijn, maatschappelijke dienstverlening, kunst en cultuur, sport, sociaal-cultureel werk of onderwijs;                 overdekt winkelcentrum;
-evenementenhal;
-congrescentrum;
-luchthaven; 
-ruimte bestemd voor passagiers die gebruik maken van middelen voor personenvervoer. 
-ruimte, gebouw of inrichting waar een werknemer zijn werkzaamheden verricht/pleegt te verrichten;                                                  horeca-inrichtingen;                  middelen van personenvervoer; vliegtuigen tijdens gebruik voor burgerluchtvaart op vluchten van en naar op Nederlands grondgebied gelegen luchthavens.    </t>
-  </si>
-  <si>
     <t xml:space="preserve">Vereisten rookruimte:   - aangewezen en  aangeduid voor het roken van tabakproducten              - afsluitbare ruimte          - geen rookoverlast in aangrenzende ruimte(n)                            - geen werkzaamheden           </t>
   </si>
   <si>
@@ -64,18 +31,7 @@
     <t xml:space="preserve">Vereisten rookruimte:  - aangewezen en  aangeduid voor het roken van tabakproducten               - afsluitbare ruimte         - geen rookoverlast in aangrenzende ruimte(n)                             - geen werkzaamheden           </t>
   </si>
   <si>
-    <t xml:space="preserve">Door de Staat of ander openbaar lichaam beheerde gebouwen of inrichtingen;                                              gebouwen of inrichtingen voor de gezondheidszorg, welzijn, maatschappelijke dienstverlening, kunst en cultuur, sport, sociaal-cultureel werk of onderwijs;                 overdekt winkelcentrum;
-evenementenhal;
-congrescentrum;
-luchthaven; 
-ruimte bestemd voor passagiers die gebruik maken van middelen voor personenvervoer. 
-ruimte, gebouw of inrichting waar een werknemer zijn werkzaamheden verricht/pleegt te verrichten;                                                 horeca-inrichtingen;                        middelen van personenvervoer; vliegtuigen tijdens gebruik voor burgerluchtvaart op vluchten van en naar op Nederlands grondgebied gelegen luchthavens.    </t>
-  </si>
-  <si>
     <t xml:space="preserve">Vereisten rookruimte:  - aangewezen en  aangeduid voor het roken van tabakproducten              - afsluitbare ruimte         - geen rookoverlast in aangrenzende ruimte(n)                            - geen werkzaamheden           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">overtreding        </t>
   </si>
   <si>
     <t>SW nalevingshulp</t>
@@ -115,9 +71,6 @@
     <t>wettelijke norm</t>
   </si>
   <si>
-    <t xml:space="preserve">Omschrijving afwijking / overtreding </t>
-  </si>
-  <si>
     <t>% of hoogte van de afwijking / interventiegrens</t>
   </si>
   <si>
@@ -140,9 +93,6 @@
   </si>
   <si>
     <t>Tabakswet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N.B (optioneel) herinspectie: herinspectie indien schriftelijke afhandeling niet heeft geleid tot adequate opheffing van de overtreding </t>
   </si>
   <si>
     <t>N.B In geval van excessen kan afgeweken worden van vastgestelde maatregelgrenzen</t>
@@ -384,9 +334,6 @@
     <t>B</t>
   </si>
   <si>
-    <t xml:space="preserve">C </t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
@@ -475,9 +422,6 @@
   </si>
   <si>
     <t xml:space="preserve">het bedrijfsmatig verstrekken of daartoe aanwezig te hebben van tabaksproducten, bestemd voor oraal gebruik anders dan roken of pruimen, in de vorm van poeder, fijne deeltjes of een combinatie van deze vormen dan wel in vormen die eruitzien als levensmiddelen   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ernstige overtreding </t>
   </si>
   <si>
     <t xml:space="preserve">herinspectie: 
@@ -620,9 +564,6 @@
 aanwezigheid rokende personen, het zien en/of ruiken van tabaksrook, aanwezigheid van asbakken gevuld met as en/of peuken van sigaren of sigaretten, 
 aanwezigheid van als asbak fungerende voorwerpen gevuld met as en/of peuken van sigaren of sigaretten, 
 aanwezigheid van sigaren- of sigarettenpeuken op de grond.    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ernstige overtreding        </t>
   </si>
   <si>
     <t>Een niet-afsluitbare rookruimte is niet aan te merken als rookruimte. Het roken in een dergelijke ruimte is dus niet toegestaan.</t>
@@ -692,9 +633,6 @@
     <t>tabaksproducent, tabaksimporteur</t>
   </si>
   <si>
-    <t>[Artikel,]</t>
-  </si>
-  <si>
     <t>artikel</t>
   </si>
   <si>
@@ -792,12 +730,63 @@
   </si>
   <si>
     <t>het gehalte aan teer, nicotine, koolmonoxide en andere stoffen die tabaksproducten, opgesplitst naar merk en type per eenheid product, voortbrengen, alsook om de gevolgen van deze andere stoffen voor de gezondheid na te gaan, daarbij onder meer rekening houdend met het inherente gevaar van afhankelijkheid.</t>
+  </si>
+  <si>
+    <t>norm</t>
+  </si>
+  <si>
+    <t>Tekst</t>
+  </si>
+  <si>
+    <t>overschrijding</t>
+  </si>
+  <si>
+    <t>ernst</t>
+  </si>
+  <si>
+    <t>klasse</t>
+  </si>
+  <si>
+    <t>motivatie</t>
+  </si>
+  <si>
+    <t>interventie</t>
+  </si>
+  <si>
+    <t>InterventieSoort</t>
+  </si>
+  <si>
+    <t>followup</t>
+  </si>
+  <si>
+    <t>opmerking</t>
+  </si>
+  <si>
+    <t>uitzoeken</t>
+  </si>
+  <si>
+    <t>Door de Staat beheerd gebouw of inrichting</t>
+  </si>
+  <si>
+    <t>[Rechtspersoon,]</t>
+  </si>
+  <si>
+    <t>[OvertredingsKlasse,]</t>
+  </si>
+  <si>
+    <t>[OvertredingsErnst,]</t>
+  </si>
+  <si>
+    <t>N.B (optioneel) herinspectie: herinspectie indien schriftelijke afhandeling niet heeft geleid tot adequate opheffing van de overtreding</t>
+  </si>
+  <si>
+    <t>Omschrijving afwijking / overtreding</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -1002,6 +991,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -1020,23 +1015,68 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>16</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>18</xdr:row>
+          <xdr:rowOff>1924050</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>17</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>19</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1028" name="Object 4" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1028"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-thema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Kantoor">
       <a:dk1>
@@ -1110,6 +1150,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1144,6 +1185,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -1319,51 +1361,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R45"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="75" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="8.75" style="9" customWidth="1"/>
-    <col min="2" max="2" width="17.75" style="13" customWidth="1"/>
-    <col min="3" max="3" width="14.125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="8.25" style="18" customWidth="1"/>
-    <col min="5" max="9" width="28.25" style="13" customWidth="1"/>
-    <col min="10" max="10" width="18.75" style="13" customWidth="1"/>
-    <col min="11" max="11" width="37.875" style="13" customWidth="1"/>
-    <col min="12" max="12" width="28.75" style="13" customWidth="1"/>
-    <col min="13" max="14" width="21.75" style="13" customWidth="1"/>
-    <col min="15" max="15" width="26.875" style="13" customWidth="1"/>
-    <col min="16" max="16" width="21.875" style="13" customWidth="1"/>
-    <col min="17" max="17" width="25.75" style="13" customWidth="1"/>
-    <col min="18" max="18" width="47.875" style="13" customWidth="1"/>
-    <col min="19" max="16384" width="9.125" style="13"/>
+    <col min="1" max="1" width="8.7109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" style="13" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" style="18" customWidth="1"/>
+    <col min="5" max="9" width="28.28515625" style="13" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" style="13" customWidth="1"/>
+    <col min="11" max="11" width="37.85546875" style="13" customWidth="1"/>
+    <col min="12" max="12" width="28.7109375" style="13" customWidth="1"/>
+    <col min="13" max="14" width="21.7109375" style="13" customWidth="1"/>
+    <col min="15" max="15" width="26.85546875" style="13" customWidth="1"/>
+    <col min="16" max="16" width="21.85546875" style="13" customWidth="1"/>
+    <col min="17" max="17" width="25.7109375" style="13" customWidth="1"/>
+    <col min="18" max="18" width="47.85546875" style="13" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="9" customFormat="1" ht="66" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="27" t="s">
-        <v>159</v>
-      </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="28"/>
+      <c r="B1" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="30"/>
       <c r="F1" s="26"/>
       <c r="G1" s="26"/>
       <c r="H1" s="26"/>
       <c r="I1" s="26"/>
       <c r="J1" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -1375,155 +1417,191 @@
     </row>
     <row r="2" spans="1:18" s="10" customFormat="1">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B2" s="5"/>
-      <c r="C2" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="29"/>
+      <c r="C2" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="31"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-      <c r="K2" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29"/>
+      <c r="K2" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
     </row>
     <row r="3" spans="1:18" s="10" customFormat="1" ht="50.25" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="R3" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:18" s="10" customFormat="1" ht="50.25" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
+        <v>179</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="5" spans="1:18" s="10" customFormat="1" ht="50.25" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D5" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>201</v>
-      </c>
       <c r="G5" s="3" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
+        <v>180</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="6" spans="1:18" s="10" customFormat="1" ht="50.25" customHeight="1">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
-      <c r="D6" s="33"/>
+      <c r="D6" s="27"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -1541,200 +1619,200 @@
     </row>
     <row r="7" spans="1:18" s="7" customFormat="1" ht="110.25" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>32</v>
+        <v>226</v>
       </c>
       <c r="R7" s="7" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:18" s="7" customFormat="1" ht="110.25" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="O8" s="1"/>
       <c r="P8" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:18" s="7" customFormat="1" ht="110.25" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="C9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="R9" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="M9" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="N9" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="P9" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q9" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="R9" s="7" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:18" s="10" customFormat="1" ht="74.25" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="O10" s="1"/>
       <c r="P10" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:18" s="10" customFormat="1" ht="74.25" customHeight="1">
       <c r="A11" s="1"/>
       <c r="B11" s="7"/>
       <c r="C11" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="1" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="I11" s="1"/>
-      <c r="J11" s="34" t="s">
-        <v>222</v>
+      <c r="J11" s="28" t="s">
+        <v>210</v>
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -1747,19 +1825,19 @@
     </row>
     <row r="12" spans="1:18" s="10" customFormat="1" ht="57" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D12" s="16">
         <v>5.2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -1767,43 +1845,43 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="L12" s="1"/>
       <c r="M12" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:18" s="10" customFormat="1" ht="55.5" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D13" s="16">
         <v>5.0999999999999996</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -1811,43 +1889,43 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="L13" s="1"/>
       <c r="M13" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:18" s="10" customFormat="1" ht="62.25" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -1855,43 +1933,43 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="R14" s="1"/>
     </row>
     <row r="15" spans="1:18" s="10" customFormat="1" ht="62.25" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D15" s="16">
         <v>5.5</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -1899,41 +1977,41 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="L15" s="1"/>
       <c r="M15" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="R15" s="1"/>
     </row>
     <row r="16" spans="1:18" s="10" customFormat="1" ht="75.75" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -1941,43 +2019,43 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="L16" s="1"/>
       <c r="M16" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:18" s="10" customFormat="1" ht="75.75" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -1985,43 +2063,43 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="L17" s="1"/>
       <c r="M17" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:18" s="10" customFormat="1" ht="73.5" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -2029,41 +2107,41 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="L18" s="1"/>
       <c r="M18" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="R18" s="1"/>
     </row>
     <row r="19" spans="1:18" s="10" customFormat="1" ht="201" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D19" s="16">
         <v>8.1</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -2071,41 +2149,41 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="L19" s="1"/>
       <c r="M19" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="R19" s="1"/>
     </row>
     <row r="20" spans="1:18" s="10" customFormat="1" ht="58.5" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D20" s="16">
         <v>8.3000000000000007</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -2113,45 +2191,45 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:18" s="10" customFormat="1" ht="60.75" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D21" s="16">
         <v>9.1</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -2159,41 +2237,41 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="L21" s="1"/>
       <c r="M21" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="R21" s="1"/>
     </row>
     <row r="22" spans="1:18" s="10" customFormat="1" ht="64.5" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D22" s="16">
         <v>9.1999999999999993</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -2201,41 +2279,41 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="L22" s="1"/>
       <c r="M22" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="R22" s="1"/>
     </row>
     <row r="23" spans="1:18" s="10" customFormat="1" ht="66.75" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D23" s="16">
         <v>9.3000000000000007</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -2243,43 +2321,43 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="R23" s="1"/>
     </row>
     <row r="24" spans="1:18" s="10" customFormat="1" ht="59.25" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D24" s="16">
         <v>9.4</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -2287,43 +2365,43 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="L24" s="1"/>
       <c r="M24" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:18" s="10" customFormat="1" ht="121.5" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D25" s="16">
         <v>9.4</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
@@ -2331,43 +2409,43 @@
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="L25" s="1"/>
       <c r="M25" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:18" s="10" customFormat="1" ht="66.75" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D26" s="16">
         <v>9.4</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -2375,43 +2453,43 @@
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="L26" s="1"/>
       <c r="M26" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:18" s="10" customFormat="1" ht="78" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D27" s="16">
         <v>9.4</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
@@ -2419,797 +2497,803 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="L27" s="1"/>
       <c r="M27" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:18" s="10" customFormat="1" ht="379.5" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>3</v>
+        <v>222</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>130</v>
+        <v>34</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
     </row>
     <row r="29" spans="1:18" s="10" customFormat="1" ht="364.5" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>3</v>
+        <v>222</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="R29" s="1"/>
     </row>
     <row r="30" spans="1:18" s="23" customFormat="1" ht="342.75" customHeight="1">
       <c r="A30" s="20" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D30" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="E30" s="20" t="s">
-        <v>3</v>
+        <v>144</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>222</v>
       </c>
       <c r="F30" s="20"/>
       <c r="G30" s="20"/>
       <c r="H30" s="20"/>
       <c r="I30" s="20"/>
       <c r="J30" s="20" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="K30" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="L30" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="M30" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="N30" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="O30" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="P30" s="20" t="s">
         <v>160</v>
       </c>
-      <c r="L30" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="M30" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="N30" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="O30" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="P30" s="20" t="s">
-        <v>170</v>
-      </c>
       <c r="Q30" s="20" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="R30" s="20" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
     </row>
     <row r="31" spans="1:18" s="10" customFormat="1" ht="384.75" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>4</v>
+        <v>222</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>172</v>
+        <v>34</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
     </row>
     <row r="32" spans="1:18" s="23" customFormat="1" ht="366" customHeight="1">
       <c r="A32" s="20" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="B32" s="21"/>
-      <c r="C32" s="20"/>
+      <c r="C32" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="D32" s="22" t="s">
-        <v>158</v>
-      </c>
-      <c r="E32" s="25" t="s">
-        <v>8</v>
+        <v>148</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>222</v>
       </c>
       <c r="F32" s="25"/>
       <c r="G32" s="25"/>
       <c r="H32" s="25"/>
       <c r="I32" s="25"/>
       <c r="J32" s="20" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K32" s="20" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="L32" s="20" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="M32" s="20" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="N32" s="20" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="O32" s="20" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="P32" s="20" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="Q32" s="20" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="R32" s="20" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
     </row>
     <row r="33" spans="1:18" s="10" customFormat="1" ht="346.5" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="E33" s="19" t="s">
-        <v>8</v>
+        <v>147</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>222</v>
       </c>
       <c r="F33" s="19"/>
       <c r="G33" s="19"/>
       <c r="H33" s="19"/>
       <c r="I33" s="19"/>
       <c r="J33" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="R33" s="1"/>
     </row>
     <row r="34" spans="1:18" s="10" customFormat="1" ht="354" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="E34" s="14" t="s">
-        <v>0</v>
+        <v>147</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>222</v>
       </c>
       <c r="F34" s="14"/>
       <c r="G34" s="14"/>
       <c r="H34" s="14"/>
       <c r="I34" s="14"/>
       <c r="J34" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="K34" s="20" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="R34" s="1"/>
     </row>
     <row r="35" spans="1:18" s="23" customFormat="1" ht="354" customHeight="1">
       <c r="A35" s="20" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>157</v>
-      </c>
-      <c r="E35" s="24" t="s">
-        <v>0</v>
+        <v>147</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>222</v>
       </c>
       <c r="F35" s="24"/>
       <c r="G35" s="24"/>
       <c r="H35" s="24"/>
       <c r="I35" s="24"/>
       <c r="J35" s="20" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="K35" s="20" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="L35" s="20"/>
       <c r="M35" s="20" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="N35" s="20" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="O35" s="20" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="P35" s="20" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="Q35" s="20" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="R35" s="20" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="36" spans="1:18" s="10" customFormat="1" ht="366" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E36" s="14" t="s">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>222</v>
       </c>
       <c r="F36" s="14"/>
       <c r="G36" s="14"/>
       <c r="H36" s="14"/>
       <c r="I36" s="14"/>
       <c r="J36" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="L36" s="1"/>
       <c r="M36" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="R36" s="1"/>
     </row>
     <row r="37" spans="1:18" s="23" customFormat="1" ht="366" customHeight="1">
       <c r="A37" s="20" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B37" s="21"/>
-      <c r="C37" s="20"/>
+      <c r="C37" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="D37" s="22" t="s">
-        <v>158</v>
-      </c>
-      <c r="E37" s="25" t="s">
-        <v>8</v>
+        <v>148</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>222</v>
       </c>
       <c r="F37" s="25"/>
       <c r="G37" s="25"/>
       <c r="H37" s="25"/>
       <c r="I37" s="25"/>
       <c r="J37" s="20" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K37" s="20" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="L37" s="20"/>
       <c r="M37" s="20" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="N37" s="20" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="O37" s="20" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="P37" s="20" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="Q37" s="20" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="R37" s="20" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
     </row>
     <row r="38" spans="1:18" s="10" customFormat="1" ht="354" customHeight="1">
       <c r="A38" s="1" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="E38" s="19" t="s">
-        <v>8</v>
+        <v>148</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>222</v>
       </c>
       <c r="F38" s="19"/>
       <c r="G38" s="19"/>
       <c r="H38" s="19"/>
       <c r="I38" s="19"/>
       <c r="J38" s="1" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="L38" s="1"/>
       <c r="M38" s="1" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="Q38" s="1" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="R38" s="1"/>
     </row>
     <row r="39" spans="1:18" s="10" customFormat="1" ht="354" customHeight="1">
       <c r="A39" s="1" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="E39" s="19" t="s">
-        <v>8</v>
+        <v>148</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>222</v>
       </c>
       <c r="F39" s="19"/>
       <c r="G39" s="19"/>
       <c r="H39" s="19"/>
       <c r="I39" s="19"/>
       <c r="J39" s="1" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="L39" s="1"/>
       <c r="M39" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="Q39" s="1" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="R39" s="1"/>
     </row>
-    <row r="40" spans="1:18" s="10" customFormat="1" ht="92.4">
+    <row r="40" spans="1:18" s="10" customFormat="1" ht="89.25">
       <c r="A40" s="1" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D40" s="16"/>
-      <c r="E40" s="1" t="s">
-        <v>40</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
+      <c r="H40" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="I40" s="1"/>
       <c r="J40" s="1" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="K40" s="8" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="L40" s="8" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="O40" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="R40" s="1" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:18" s="10" customFormat="1" ht="63" customHeight="1">
       <c r="A41" s="1" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D41" s="16">
         <v>3.1</v>
       </c>
-      <c r="E41" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
+      <c r="H41" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="N41" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="O41" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="Q41" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="R41" s="1" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:18" s="10" customFormat="1" ht="66.75" customHeight="1">
       <c r="A42" s="1" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>94</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
+      <c r="H42" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="N42" s="1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="O42" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="P42" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="Q42" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="R42" s="1" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="43" spans="1:18" s="10" customFormat="1" ht="66.75" customHeight="1">
       <c r="A43" s="1" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D43" s="16">
         <v>3.1</v>
       </c>
-      <c r="E43" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
+      <c r="H43" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="N43" s="1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="O43" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="R43" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" s="10" customFormat="1" ht="105.6">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" s="10" customFormat="1" ht="89.25">
       <c r="A44" s="1" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>40</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
+      <c r="H44" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="L44" s="1"/>
       <c r="M44" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="N44" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="O44" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="P44" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="Q44" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="R44" s="1"/>
     </row>
@@ -3224,16 +3308,16 @@
       <c r="H45" s="11"/>
       <c r="I45" s="11"/>
       <c r="J45" s="11"/>
-      <c r="K45" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="L45" s="31"/>
-      <c r="M45" s="31"/>
-      <c r="N45" s="31"/>
-      <c r="O45" s="31"/>
-      <c r="P45" s="31"/>
-      <c r="Q45" s="31"/>
-      <c r="R45" s="32"/>
+      <c r="K45" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="L45" s="33"/>
+      <c r="M45" s="33"/>
+      <c r="N45" s="33"/>
+      <c r="O45" s="33"/>
+      <c r="P45" s="33"/>
+      <c r="Q45" s="33"/>
+      <c r="R45" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3249,9 +3333,34 @@
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="32" max="13" man="1"/>
   </rowBreaks>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <oleObjects>
-    <oleObject progId="Outlook.FileAttach" shapeId="1028" r:id="rId3"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Outlook.FileAttach" shapeId="1028" r:id="rId4">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>16</xdr:col>
+                <xdr:colOff>266700</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>1924050</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>17</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>19</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Outlook.FileAttach" shapeId="1028" r:id="rId4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
   </oleObjects>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Make Arch.adl generate a prototype
</commit_message>
<xml_diff>
--- a/Blik/Interventiebeleid tabak.xlsx
+++ b/Blik/Interventiebeleid tabak.xlsx
@@ -10,17 +10,14 @@
     <sheet name="Specifiek" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Specifiek!$A$1:$R$45</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Specifiek!$A$1:$R$63</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="228">
-  <si>
-    <t>10.1 a;    10.1 b;     10.1 c;     10.1 d;    10.1 e;     10.1 f;     10.1 g.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="270">
   <si>
     <t xml:space="preserve">Vereisten rookruimte:   - aangewezen en  aangeduid voor het roken van tabakproducten              - afsluitbare ruimte          - geen rookoverlast in aangrenzende ruimte(n)                            - geen werkzaamheden           </t>
   </si>
@@ -143,9 +140,6 @@
     <t xml:space="preserve">uitzonderingen: art. 5,2 en 5.3 en juridisch vastgelegd in beleidsnotities.   </t>
   </si>
   <si>
-    <t>3 e</t>
-  </si>
-  <si>
     <t>elke vorme van reclame die de suggestie wekken dat een bepaald tabaksproduct minder schadelijk is dan een ander tabaksproduct</t>
   </si>
   <si>
@@ -158,27 +152,18 @@
     <t>BR, nalevingshulp</t>
   </si>
   <si>
-    <t>5a, 1</t>
-  </si>
-  <si>
     <t xml:space="preserve">verbod om een naam of merk etc. van een ander product te gebruiken voor een tabaksproduct </t>
   </si>
   <si>
     <t>Tenzij dit tabaksproduct reeds vóór de datum van inwerkingtreding van het in art. 5.1 bedoelde verbod onder die naam, dat merk of symbool, dan wel met dat onderscheidende teken, in de handel was.</t>
   </si>
   <si>
-    <t>5a, 2</t>
-  </si>
-  <si>
     <t>verbod om een naam of merk etc. van een tabaksproduct te gebruiken voor een ander product</t>
   </si>
   <si>
     <t>Tenzij de naam , het merk, het symbool of het andere onderscheidende teken van het product of de dienst in een duidelijk andere vorm dan die van het tabaksproduct wordt gepresenteerd.</t>
   </si>
   <si>
-    <t>7,1 7,2</t>
-  </si>
-  <si>
     <t>verkoop van tabaksproducten in inrichtingen waar dit niet is toegestaan</t>
   </si>
   <si>
@@ -234,9 +219,6 @@
   </si>
   <si>
     <t>verstrekken van tabaksproducten vanuit een automaat die niet in het zicht van de exploitant of het personeel staat</t>
-  </si>
-  <si>
-    <t>instellen, aanduiden, handhaven rookverbod</t>
   </si>
   <si>
     <t>BR nalevingshulp</t>
@@ -412,13 +394,7 @@
     <t>afwijkingen aanduidingen op verpakkingen tabaksproducten gerelateerd aan schadelijkheid.</t>
   </si>
   <si>
-    <t>5.4c, sub 3</t>
-  </si>
-  <si>
     <t>NVWA -maatregel</t>
-  </si>
-  <si>
-    <t>3a</t>
   </si>
   <si>
     <t xml:space="preserve">het bedrijfsmatig verstrekken of daartoe aanwezig te hebben van tabaksproducten, bestemd voor oraal gebruik anders dan roken of pruimen, in de vorm van poeder, fijne deeltjes of een combinatie van deze vormen dan wel in vormen die eruitzien als levensmiddelen   </t>
@@ -504,24 +480,12 @@
 aanwezigheid van sigaren- of sigarettenpeuken op de grond.                   </t>
   </si>
   <si>
-    <t>10.1 a;     10.1 b;      10.1 c;      10.1 d;     10.1 e;      10.1 f;      10.1 g.</t>
-  </si>
-  <si>
     <t xml:space="preserve">De rookruimte is niet afsluitbaar en er wordt/is gerookt in de rookruimte hetgeen blijkt uit bijv: 
 aanwezigheid rokende personen, het zien en/of ruiken van tabaksrook, aanwezigheid van asbakken gevuld met as en/of peuken van sigaren of sigaretten, 
 aanwezigheid van als asbak fungerende voorwerpen gevuld met as en/of peuken van sigaren of sigaretten, 
 aanwezigheid van sigaren- of sigarettenpeuken op de grond.                   </t>
   </si>
   <si>
-    <t>10.1 a;    10.1 b;    10.1 c;    10.1 d;    10.1 e;     10.1 f;      10.1 g.</t>
-  </si>
-  <si>
-    <t>10.1 a;    10.1 b;    10.1 c;    10.1 d;    10.1 e;    10.1 f;     10.1 g.</t>
-  </si>
-  <si>
-    <t>10.1 a;    10.1 b;    10.1 c;    10.1 d;     10.1 e;    10.1 f;     10.1 g.</t>
-  </si>
-  <si>
     <t>Specifiek interventiebeleid tabak: Overzicht specifieke interventies NVWA m.b.t. tabak, bijlage bij IB02-SPEC31 Interventiebeleid tabak, versie 5</t>
   </si>
   <si>
@@ -532,9 +496,6 @@
   </si>
   <si>
     <t>geringe overtreding</t>
-  </si>
-  <si>
-    <t>Risico Volksgezondheid</t>
   </si>
   <si>
     <t>D</t>
@@ -672,9 +633,6 @@
     <t>eisen krachtens artikel 2 Tabakswet</t>
   </si>
   <si>
-    <t>3 lid 1</t>
-  </si>
-  <si>
     <t>plicht</t>
   </si>
   <si>
@@ -687,21 +645,12 @@
     <t>lijst van alle ingrediënten, met opgave van de hoeveelheden, die voor de productie van hun tabaksproducten worden gebruikt, opgesplitst naar merk en type per eenheid product</t>
   </si>
   <si>
-    <t>3b lid 1</t>
-  </si>
-  <si>
-    <t>3b lid 2</t>
-  </si>
-  <si>
     <t>verklaring waarin wordt uiteengezet waarom de ingrediënten aan de tabaksproducten worden toegevoegd</t>
   </si>
   <si>
     <t>De functie en de categorie van elk ingredient worden vermeld. Bij de lijst gaan tevens de voor de producent of de importeur beschikbare toxicologische gegevens betreffende de ingrediënten in verbrande en onverbrande vorm, naar gelang van het geval, waarbij in het bijzonder de gevolgen daarvan voor de gezondheid worden vermeld en mogelijke verslavende effecten in aanmerking worden genomen. De lijst wordt opgesteld in afnemende volgorde naar gewicht van de respectieve ingrediënten van het product.</t>
   </si>
   <si>
-    <t>3c lid 1</t>
-  </si>
-  <si>
     <t>medewerking verlenen</t>
   </si>
   <si>
@@ -762,9 +711,6 @@
     <t>opmerking</t>
   </si>
   <si>
-    <t>uitzoeken</t>
-  </si>
-  <si>
     <t>Door de Staat beheerd gebouw of inrichting</t>
   </si>
   <si>
@@ -781,6 +727,186 @@
   </si>
   <si>
     <t>Omschrijving afwijking / overtreding</t>
+  </si>
+  <si>
+    <t>Art. 10 lid 1 sub a</t>
+  </si>
+  <si>
+    <t>orgaan</t>
+  </si>
+  <si>
+    <t>rookverbod</t>
+  </si>
+  <si>
+    <t>in een gebouw of inrichting, dat onderscheidenlijk die bij de Staat of een ander openbaar lichaam in gebruik is</t>
+  </si>
+  <si>
+    <t>instellen</t>
+  </si>
+  <si>
+    <t>aanduiden</t>
+  </si>
+  <si>
+    <t>handhaven</t>
+  </si>
+  <si>
+    <t>Art. 10 lid 1 sub b</t>
+  </si>
+  <si>
+    <t>IB 02 SPEC 31, regel 19b</t>
+  </si>
+  <si>
+    <t>IB 02 SPEC 31, regel 31b</t>
+  </si>
+  <si>
+    <t>IB 02 SPEC 31, regel 18 b</t>
+  </si>
+  <si>
+    <t>in een gebouw of inrichting, dat onderscheidenlijk die in gebruik is bij een instelling of vereniging voor gezondheidszorg, welzijn, maatschappelijke dienstverlening, kunst en cultuur, sport, sociaal-cultureel werk of onderwijs</t>
+  </si>
+  <si>
+    <t>beheerder</t>
+  </si>
+  <si>
+    <t>in een ruimte, gebouw of inrichting waar een werknemer zijn werkzaamheden verricht of pleegt te verrichten</t>
+  </si>
+  <si>
+    <t>werkgever</t>
+  </si>
+  <si>
+    <t>Art. 10 lid 1 sub c</t>
+  </si>
+  <si>
+    <t>IB 02 SPEC 31, regel 18 c</t>
+  </si>
+  <si>
+    <t>IB 02 SPEC 31, regel 31c</t>
+  </si>
+  <si>
+    <t>IB 02 SPEC 31, regel 19c</t>
+  </si>
+  <si>
+    <t>in andere bij algemene maatregel van bestuur aan te wijzen gebouwen of inrichtingen of delen daarvan</t>
+  </si>
+  <si>
+    <t>Art. 10 lid 1 sub d</t>
+  </si>
+  <si>
+    <t>IB 02 SPEC 31, regel 18 d</t>
+  </si>
+  <si>
+    <t>IB 02 SPEC 31, regel 31d</t>
+  </si>
+  <si>
+    <t>IB 02 SPEC 31, regel 19d</t>
+  </si>
+  <si>
+    <t>in een horeca-inrichting</t>
+  </si>
+  <si>
+    <t>Art. 10 lid 1 sub e</t>
+  </si>
+  <si>
+    <t>IB 02 SPEC 31, regel 18 e</t>
+  </si>
+  <si>
+    <t>IB 02 SPEC 31, regel 31e</t>
+  </si>
+  <si>
+    <t>IB 02 SPEC 31, regel 19e</t>
+  </si>
+  <si>
+    <t>exploitant</t>
+  </si>
+  <si>
+    <t>in een middel voor personenvervoer</t>
+  </si>
+  <si>
+    <t>Art. 10 lid 1 sub f</t>
+  </si>
+  <si>
+    <t>IB 02 SPEC 31, regel 18f</t>
+  </si>
+  <si>
+    <t>IB 02 SPEC 31, regel 31f</t>
+  </si>
+  <si>
+    <t>IB 02 SPEC 31, regel 19f</t>
+  </si>
+  <si>
+    <t>ondernemer</t>
+  </si>
+  <si>
+    <t>in een vliegtuig tijdens gebruik voor burgerluchtvaart op vluchten van en naar op Nederlands grondgebied gelegen luchthavens</t>
+  </si>
+  <si>
+    <t>Art. 10 lid 1 sub g</t>
+  </si>
+  <si>
+    <t>IB 02 SPEC 31, regel 18g</t>
+  </si>
+  <si>
+    <t>IB 02 SPEC 31, regel 31g</t>
+  </si>
+  <si>
+    <t>IB 02 SPEC 31, regel 19g</t>
+  </si>
+  <si>
+    <t>Art. 3 lid 1</t>
+  </si>
+  <si>
+    <t>Art. 3b lid 1</t>
+  </si>
+  <si>
+    <t>Art. 3b lid 2</t>
+  </si>
+  <si>
+    <t>Art. 3c lid 1</t>
+  </si>
+  <si>
+    <t>Art. 5 lid 2</t>
+  </si>
+  <si>
+    <t>Art. 5 lid 1</t>
+  </si>
+  <si>
+    <t>Art. 5 lid 5</t>
+  </si>
+  <si>
+    <t>Art. 5a lid 1</t>
+  </si>
+  <si>
+    <t>Art. 5a lid 2</t>
+  </si>
+  <si>
+    <t>Art. 7 lid 1, Art. 7 lid 2</t>
+  </si>
+  <si>
+    <t>Art. 8 lid 1</t>
+  </si>
+  <si>
+    <t>Art. 8 lid 3</t>
+  </si>
+  <si>
+    <t>Art. 9 lid 1</t>
+  </si>
+  <si>
+    <t>Art. 9 lid 2</t>
+  </si>
+  <si>
+    <t>Art. 9 lid 3</t>
+  </si>
+  <si>
+    <t>Art. 9 lid 4</t>
+  </si>
+  <si>
+    <t>Art. 3a</t>
+  </si>
+  <si>
+    <t>Art. 3e</t>
+  </si>
+  <si>
+    <t>Art. 5 lid 4 sub c.3</t>
   </si>
 </sst>
 </file>
@@ -1362,13 +1488,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R45"/>
+  <dimension ref="A1:R63"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="75" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="K1" zoomScale="75" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -1392,7 +1516,7 @@
     <row r="1" spans="1:18" s="9" customFormat="1" ht="66" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="29" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="C1" s="29"/>
       <c r="D1" s="29"/>
@@ -1402,10 +1526,10 @@
       <c r="H1" s="26"/>
       <c r="I1" s="26"/>
       <c r="J1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -1417,11 +1541,11 @@
     </row>
     <row r="2" spans="1:18" s="10" customFormat="1">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="31"/>
       <c r="E2" s="2"/>
@@ -1431,7 +1555,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="31" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="L2" s="31"/>
       <c r="M2" s="31"/>
@@ -1443,158 +1567,158 @@
     </row>
     <row r="3" spans="1:18" s="10" customFormat="1" ht="50.25" customHeight="1">
       <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="E3" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="R3" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:18" s="10" customFormat="1" ht="50.25" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>188</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>219</v>
+        <v>202</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5" spans="1:18" s="10" customFormat="1" ht="50.25" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="15" t="s">
-        <v>14</v>
-      </c>
       <c r="E5" s="3" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:18" s="10" customFormat="1" ht="50.25" customHeight="1">
@@ -1619,200 +1743,200 @@
     </row>
     <row r="7" spans="1:18" s="7" customFormat="1" ht="110.25" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q7" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="R7" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="Q7" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="R7" s="7" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:18" s="7" customFormat="1" ht="110.25" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>205</v>
+        <v>188</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>196</v>
+        <v>252</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="L8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="M8" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="N8" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="O8" s="1"/>
       <c r="P8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="R8" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:18" s="7" customFormat="1" ht="110.25" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>206</v>
+        <v>189</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>197</v>
+        <v>253</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="L9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="M9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="M9" s="7" t="s">
+      <c r="N9" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="P9" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="N9" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="P9" s="7" t="s">
+      <c r="Q9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="Q9" s="7" t="s">
+      <c r="R9" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="R9" s="7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:18" s="10" customFormat="1" ht="74.25" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>207</v>
+        <v>190</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>200</v>
+        <v>254</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>201</v>
+        <v>184</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>202</v>
+        <v>185</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1" t="s">
-        <v>203</v>
+        <v>186</v>
       </c>
       <c r="L10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="M10" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="N10" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="O10" s="1"/>
       <c r="P10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="R10" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:18" s="10" customFormat="1" ht="74.25" customHeight="1">
       <c r="A11" s="1"/>
       <c r="B11" s="7"/>
       <c r="C11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>200</v>
+        <v>254</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>208</v>
+        <v>191</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="1" t="s">
-        <v>209</v>
+        <v>192</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="28" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -1825,19 +1949,19 @@
     </row>
     <row r="12" spans="1:18" s="10" customFormat="1" ht="57" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="16">
-        <v>5.2</v>
+        <v>23</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>255</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -1845,43 +1969,43 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L12" s="1"/>
       <c r="M12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="O12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N12" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="O12" s="1" t="s">
+      <c r="P12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="P12" s="1" t="s">
+      <c r="Q12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Q12" s="1" t="s">
+      <c r="R12" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:18" s="10" customFormat="1" ht="55.5" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="16">
-        <v>5.0999999999999996</v>
+        <v>23</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>256</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -1889,43 +2013,43 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L13" s="1"/>
       <c r="M13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="O13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N13" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="O13" s="1" t="s">
+      <c r="P13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="P13" s="1" t="s">
+      <c r="Q13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Q13" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="R13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:18" s="10" customFormat="1" ht="62.25" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>41</v>
+        <v>268</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -1933,43 +2057,43 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="M14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="O14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N14" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="O14" s="1" t="s">
+      <c r="P14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="P14" s="1" t="s">
+      <c r="Q14" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="Q14" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="R14" s="1"/>
     </row>
     <row r="15" spans="1:18" s="10" customFormat="1" ht="62.25" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="16">
-        <v>5.5</v>
+        <v>23</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>257</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -1977,41 +2101,41 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L15" s="1"/>
       <c r="M15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="O15" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N15" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="P15" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R15" s="1"/>
     </row>
     <row r="16" spans="1:18" s="10" customFormat="1" ht="75.75" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>46</v>
+        <v>258</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -2019,43 +2143,43 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L16" s="1"/>
       <c r="M16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="O16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N16" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="P16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R16" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="Q16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R16" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:18" s="10" customFormat="1" ht="75.75" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>49</v>
+        <v>259</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -2063,43 +2187,43 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="L17" s="1"/>
       <c r="M17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="O17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N17" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="P17" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:18" s="10" customFormat="1" ht="73.5" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>52</v>
+        <v>260</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -2107,41 +2231,41 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="L18" s="1"/>
       <c r="M18" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="R18" s="1"/>
     </row>
     <row r="19" spans="1:18" s="10" customFormat="1" ht="201" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="16">
-        <v>8.1</v>
+        <v>23</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>261</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -2149,41 +2273,41 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="L19" s="1"/>
       <c r="M19" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="R19" s="1"/>
     </row>
     <row r="20" spans="1:18" s="10" customFormat="1" ht="58.5" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="16">
-        <v>8.3000000000000007</v>
+        <v>23</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>262</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -2191,45 +2315,45 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="P20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R20" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="Q20" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="R20" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:18" s="10" customFormat="1" ht="60.75" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="16">
-        <v>9.1</v>
+        <v>23</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>263</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -2237,41 +2361,41 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="L21" s="1"/>
       <c r="M21" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R21" s="1"/>
     </row>
     <row r="22" spans="1:18" s="10" customFormat="1" ht="64.5" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="16">
-        <v>9.1999999999999993</v>
+        <v>23</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>264</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -2279,41 +2403,41 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="L22" s="1"/>
       <c r="M22" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R22" s="1"/>
     </row>
     <row r="23" spans="1:18" s="10" customFormat="1" ht="66.75" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" s="16">
-        <v>9.3000000000000007</v>
+        <v>23</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>265</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -2321,43 +2445,43 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R23" s="1"/>
     </row>
     <row r="24" spans="1:18" s="10" customFormat="1" ht="59.25" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" s="16">
-        <v>9.4</v>
+        <v>23</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>266</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -2365,43 +2489,43 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="L24" s="1"/>
       <c r="M24" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:18" s="10" customFormat="1" ht="121.5" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25" s="16">
-        <v>9.4</v>
+        <v>23</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>266</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
@@ -2409,43 +2533,43 @@
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="L25" s="1"/>
       <c r="M25" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:18" s="10" customFormat="1" ht="66.75" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D26" s="16">
-        <v>9.4</v>
+        <v>23</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>266</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -2453,43 +2577,43 @@
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="L26" s="1"/>
       <c r="M26" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:18" s="10" customFormat="1" ht="78" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D27" s="16">
-        <v>9.4</v>
+        <v>23</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>266</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
@@ -2497,841 +2621,1739 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="L27" s="1"/>
       <c r="M27" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" s="10" customFormat="1" ht="379.5" customHeight="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" s="10" customFormat="1" ht="78" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>26</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="B28" s="7"/>
       <c r="C28" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
+        <v>210</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="I28" s="1"/>
       <c r="J28" s="1" t="s">
-        <v>72</v>
+        <v>213</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>143</v>
+        <v>118</v>
       </c>
       <c r="M28" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="O28" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N28" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="O28" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="P28" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="R28" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" s="10" customFormat="1" ht="364.5" customHeight="1">
+        <v>36</v>
+      </c>
+      <c r="R28" s="1"/>
+    </row>
+    <row r="29" spans="1:18" s="10" customFormat="1" ht="78" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>26</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="B29" s="7"/>
       <c r="C29" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
+        <v>210</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="I29" s="1"/>
       <c r="J29" s="1" t="s">
-        <v>72</v>
+        <v>213</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>54</v>
+        <v>140</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>91</v>
+        <v>141</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P29" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="R29" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" s="10" customFormat="1" ht="78" customHeight="1">
+      <c r="A30" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B30" s="7"/>
+      <c r="C30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P30" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Q29" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R29" s="1"/>
-    </row>
-    <row r="30" spans="1:18" s="23" customFormat="1" ht="342.75" customHeight="1">
-      <c r="A30" s="20" t="s">
-        <v>168</v>
-      </c>
-      <c r="B30" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D30" s="22" t="s">
-        <v>144</v>
-      </c>
-      <c r="E30" s="1" t="s">
+      <c r="Q30" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="R30" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" s="10" customFormat="1" ht="78" customHeight="1">
+      <c r="A31" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B31" s="7"/>
+      <c r="C31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="E31" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="K30" s="20" t="s">
-        <v>150</v>
-      </c>
-      <c r="L30" s="20" t="s">
-        <v>151</v>
-      </c>
-      <c r="M30" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="N30" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="O30" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="P30" s="20" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q30" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="R30" s="20" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" s="10" customFormat="1" ht="384.75" customHeight="1">
-      <c r="A31" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D31" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
+      <c r="F31" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="I31" s="1"/>
       <c r="J31" s="1" t="s">
-        <v>2</v>
+        <v>221</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>145</v>
+        <v>118</v>
       </c>
       <c r="M31" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="O31" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N31" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="O31" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="P31" s="1" t="s">
-        <v>73</v>
+        <v>4</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R31" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" s="23" customFormat="1" ht="366" customHeight="1">
-      <c r="A32" s="20" t="s">
-        <v>169</v>
-      </c>
-      <c r="B32" s="21"/>
+        <v>36</v>
+      </c>
+      <c r="R31" s="1"/>
+    </row>
+    <row r="32" spans="1:18" s="10" customFormat="1" ht="78" customHeight="1">
+      <c r="A32" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B32" s="7"/>
       <c r="C32" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D32" s="22" t="s">
-        <v>148</v>
-      </c>
-      <c r="E32" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="E32" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="25"/>
-      <c r="I32" s="25"/>
-      <c r="J32" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="K32" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="L32" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="M32" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="N32" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="O32" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="P32" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q32" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="R32" s="20" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" s="10" customFormat="1" ht="346.5" customHeight="1">
+      <c r="F32" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q32" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="R32" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" s="10" customFormat="1" ht="78" customHeight="1">
       <c r="A33" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B33" s="7"/>
+      <c r="C33" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="E33" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="L33" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B33" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D33" s="16" t="s">
+      <c r="M33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="O33" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P33" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q33" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="R33" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" s="10" customFormat="1" ht="78" customHeight="1">
+      <c r="A34" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B34" s="7"/>
+      <c r="C34" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="E34" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P34" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q34" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R34" s="1"/>
+    </row>
+    <row r="35" spans="1:18" s="10" customFormat="1" ht="78" customHeight="1">
+      <c r="A35" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B35" s="7"/>
+      <c r="C35" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="E35" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="O35" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P35" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="Q35" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="R35" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" s="10" customFormat="1" ht="78" customHeight="1">
+      <c r="A36" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B36" s="7"/>
+      <c r="C36" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="E36" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q36" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="R36" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" s="10" customFormat="1" ht="78" customHeight="1">
+      <c r="A37" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B37" s="7"/>
+      <c r="C37" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E37" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K33" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="L33" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="M33" s="1" t="s">
+      <c r="F37" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="O37" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N33" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="O33" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="P33" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q33" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="R33" s="1"/>
-    </row>
-    <row r="34" spans="1:18" s="10" customFormat="1" ht="354" customHeight="1">
-      <c r="A34" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D34" s="16" t="s">
+      <c r="P37" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q37" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R37" s="1"/>
+    </row>
+    <row r="38" spans="1:18" s="10" customFormat="1" ht="78" customHeight="1">
+      <c r="A38" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B38" s="7"/>
+      <c r="C38" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E38" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P38" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="Q38" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="R38" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" s="10" customFormat="1" ht="78" customHeight="1">
+      <c r="A39" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B39" s="7"/>
+      <c r="C39" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E39" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K34" s="20" t="s">
-        <v>166</v>
-      </c>
-      <c r="L34" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="M34" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="N34" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="O34" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="P34" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q34" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="R34" s="1"/>
-    </row>
-    <row r="35" spans="1:18" s="23" customFormat="1" ht="354" customHeight="1">
-      <c r="A35" s="20" t="s">
-        <v>170</v>
-      </c>
-      <c r="B35" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="C35" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D35" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="F35" s="24"/>
-      <c r="G35" s="24"/>
-      <c r="H35" s="24"/>
-      <c r="I35" s="24"/>
-      <c r="J35" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="K35" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="L35" s="20"/>
-      <c r="M35" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="N35" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="O35" s="20" t="s">
-        <v>159</v>
-      </c>
-      <c r="P35" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="Q35" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="R35" s="20" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" s="10" customFormat="1" ht="366" customHeight="1">
-      <c r="A36" s="1" t="s">
+      <c r="F39" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P39" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q39" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B36" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D36" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K36" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="L36" s="1"/>
-      <c r="M36" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="N36" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="O36" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="P36" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q36" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="R36" s="1"/>
-    </row>
-    <row r="37" spans="1:18" s="23" customFormat="1" ht="366" customHeight="1">
-      <c r="A37" s="20" t="s">
-        <v>171</v>
-      </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D37" s="22" t="s">
-        <v>148</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="25"/>
-      <c r="I37" s="25"/>
-      <c r="J37" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="K37" s="20" t="s">
-        <v>165</v>
-      </c>
-      <c r="L37" s="20"/>
-      <c r="M37" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="N37" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="O37" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="P37" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q37" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="R37" s="20" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" s="10" customFormat="1" ht="354" customHeight="1">
-      <c r="A38" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D38" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="F38" s="19"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="19"/>
-      <c r="I38" s="19"/>
-      <c r="J38" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="K38" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="L38" s="1"/>
-      <c r="M38" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="N38" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="O38" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="P38" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q38" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="R38" s="1"/>
-    </row>
-    <row r="39" spans="1:18" s="10" customFormat="1" ht="354" customHeight="1">
-      <c r="A39" s="1" t="s">
+      <c r="R39" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B39" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D39" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="F39" s="19"/>
-      <c r="G39" s="19"/>
-      <c r="H39" s="19"/>
-      <c r="I39" s="19"/>
-      <c r="J39" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="K39" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="L39" s="1"/>
-      <c r="M39" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="N39" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="O39" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="P39" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q39" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="R39" s="1"/>
-    </row>
-    <row r="40" spans="1:18" s="10" customFormat="1" ht="89.25">
+    </row>
+    <row r="40" spans="1:18" s="10" customFormat="1" ht="78" customHeight="1">
       <c r="A40" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>26</v>
-      </c>
+        <v>238</v>
+      </c>
+      <c r="B40" s="7"/>
       <c r="C40" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>221</v>
-      </c>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
+        <v>235</v>
+      </c>
+      <c r="E40" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="H40" s="1" t="s">
-        <v>32</v>
+        <v>212</v>
       </c>
       <c r="I40" s="1"/>
       <c r="J40" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="O40" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P40" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q40" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R40" s="1"/>
+    </row>
+    <row r="41" spans="1:18" s="10" customFormat="1" ht="78" customHeight="1">
+      <c r="A41" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B41" s="7"/>
+      <c r="C41" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="E41" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="O41" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P41" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q41" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="R41" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" s="10" customFormat="1" ht="78" customHeight="1">
+      <c r="A42" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B42" s="7"/>
+      <c r="C42" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="O42" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P42" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q42" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="R42" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" s="10" customFormat="1" ht="78" customHeight="1">
+      <c r="A43" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B43" s="7"/>
+      <c r="C43" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D43" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="E43" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="O43" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P43" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q43" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R43" s="1"/>
+    </row>
+    <row r="44" spans="1:18" s="10" customFormat="1" ht="78" customHeight="1">
+      <c r="A44" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B44" s="7"/>
+      <c r="C44" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D44" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="E44" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="O44" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P44" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q44" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="R44" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" s="10" customFormat="1" ht="78" customHeight="1">
+      <c r="A45" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B45" s="7"/>
+      <c r="C45" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="E45" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N45" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="O45" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P45" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q45" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="R45" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" s="10" customFormat="1" ht="78" customHeight="1">
+      <c r="A46" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B46" s="7"/>
+      <c r="C46" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>247</v>
+      </c>
+      <c r="E46" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="M46" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N46" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="O46" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P46" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q46" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R46" s="1"/>
+    </row>
+    <row r="47" spans="1:18" s="10" customFormat="1" ht="78" customHeight="1">
+      <c r="A47" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B47" s="7"/>
+      <c r="C47" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D47" s="16" t="s">
+        <v>247</v>
+      </c>
+      <c r="E47" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="N47" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="O47" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P47" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q47" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="R47" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" s="10" customFormat="1" ht="78" customHeight="1">
+      <c r="A48" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B48" s="7"/>
+      <c r="C48" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>247</v>
+      </c>
+      <c r="E48" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M48" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N48" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="O48" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P48" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q48" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="R48" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" s="10" customFormat="1" ht="384.75" customHeight="1">
+      <c r="A49" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C49" s="1"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="M49" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N49" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="O49" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P49" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q49" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R49" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" s="23" customFormat="1" ht="366" customHeight="1">
+      <c r="A50" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="B50" s="21"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F50" s="25"/>
+      <c r="G50" s="25"/>
+      <c r="H50" s="25"/>
+      <c r="I50" s="25"/>
+      <c r="J50" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="K50" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="L50" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="M50" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="N50" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="O50" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="P50" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q50" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="R50" s="20" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" s="10" customFormat="1" ht="346.5" customHeight="1">
+      <c r="A51" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C51" s="1"/>
+      <c r="D51" s="16"/>
+      <c r="E51" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F51" s="19"/>
+      <c r="G51" s="19"/>
+      <c r="H51" s="19"/>
+      <c r="I51" s="19"/>
+      <c r="J51" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="M51" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N51" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="O51" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P51" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q51" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="R51" s="1"/>
+    </row>
+    <row r="52" spans="1:18" s="10" customFormat="1" ht="354" customHeight="1">
+      <c r="A52" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C52" s="1"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="14"/>
+      <c r="I52" s="14"/>
+      <c r="J52" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K52" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="M52" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N52" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="O52" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P52" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q52" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="R52" s="1"/>
+    </row>
+    <row r="53" spans="1:18" s="23" customFormat="1" ht="354" customHeight="1">
+      <c r="A53" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="B53" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C53" s="20"/>
+      <c r="D53" s="22"/>
+      <c r="E53" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F53" s="24"/>
+      <c r="G53" s="24"/>
+      <c r="H53" s="24"/>
+      <c r="I53" s="24"/>
+      <c r="J53" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="K53" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="L53" s="20"/>
+      <c r="M53" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="N53" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="O53" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="P53" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q53" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="R53" s="20" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" s="10" customFormat="1" ht="366" customHeight="1">
+      <c r="A54" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C54" s="1"/>
+      <c r="D54" s="16"/>
+      <c r="E54" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F54" s="14"/>
+      <c r="G54" s="14"/>
+      <c r="H54" s="14"/>
+      <c r="I54" s="14"/>
+      <c r="J54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L54" s="1"/>
+      <c r="M54" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N54" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="O54" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P54" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q54" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="R54" s="1"/>
+    </row>
+    <row r="55" spans="1:18" s="23" customFormat="1" ht="366" customHeight="1">
+      <c r="A55" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="B55" s="21"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="22"/>
+      <c r="E55" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F55" s="25"/>
+      <c r="G55" s="25"/>
+      <c r="H55" s="25"/>
+      <c r="I55" s="25"/>
+      <c r="J55" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="K55" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="L55" s="20"/>
+      <c r="M55" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="N55" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="O55" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="P55" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q55" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="R55" s="20" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" s="10" customFormat="1" ht="354" customHeight="1">
+      <c r="A56" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C56" s="1"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F56" s="19"/>
+      <c r="G56" s="19"/>
+      <c r="H56" s="19"/>
+      <c r="I56" s="19"/>
+      <c r="J56" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="L56" s="1"/>
+      <c r="M56" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="N56" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="O56" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P56" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q56" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="R56" s="1"/>
+    </row>
+    <row r="57" spans="1:18" s="10" customFormat="1" ht="354" customHeight="1">
+      <c r="A57" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C57" s="1"/>
+      <c r="D57" s="16"/>
+      <c r="E57" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F57" s="19"/>
+      <c r="G57" s="19"/>
+      <c r="H57" s="19"/>
+      <c r="I57" s="19"/>
+      <c r="J57" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="L57" s="1"/>
+      <c r="M57" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N57" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="O57" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P57" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q57" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="R57" s="1"/>
+    </row>
+    <row r="58" spans="1:18" s="10" customFormat="1" ht="89.25">
+      <c r="A58" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D58" s="16"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K58" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="L58" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="M58" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="N58" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="O58" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="P58" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q58" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R58" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" s="10" customFormat="1" ht="63" customHeight="1">
+      <c r="A59" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D59" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L59" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="K40" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="L40" s="8" t="s">
+      <c r="M59" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="N59" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="O59" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P59" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q59" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R59" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" s="10" customFormat="1" ht="66.75" customHeight="1">
+      <c r="A60" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D60" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="L60" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M60" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N60" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="O60" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P60" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q60" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R60" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" s="10" customFormat="1" ht="66.75" customHeight="1">
+      <c r="A61" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D61" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L61" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M61" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N61" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="O61" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P61" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q61" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R61" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="M40" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="N40" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="O40" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="P40" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q40" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R40" s="1" t="s">
+    </row>
+    <row r="62" spans="1:18" s="10" customFormat="1" ht="89.25">
+      <c r="A62" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D62" s="16" t="s">
+        <v>267</v>
+      </c>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+      <c r="K62" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="L62" s="1"/>
+      <c r="M62" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N62" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="O62" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P62" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q62" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R62" s="1"/>
+    </row>
+    <row r="63" spans="1:18" s="10" customFormat="1" ht="114.75" customHeight="1">
+      <c r="A63" s="11"/>
+      <c r="B63" s="12"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="17"/>
+      <c r="E63" s="11"/>
+      <c r="F63" s="11"/>
+      <c r="G63" s="11"/>
+      <c r="H63" s="11"/>
+      <c r="I63" s="11"/>
+      <c r="J63" s="11"/>
+      <c r="K63" s="32" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="41" spans="1:18" s="10" customFormat="1" ht="63" customHeight="1">
-      <c r="A41" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D41" s="16">
-        <v>3.1</v>
-      </c>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="L41" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="M41" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="N41" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="O41" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="P41" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q41" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R41" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" s="10" customFormat="1" ht="66.75" customHeight="1">
-      <c r="A42" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D42" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="L42" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="M42" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="N42" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="O42" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="P42" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q42" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R42" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" s="10" customFormat="1" ht="66.75" customHeight="1">
-      <c r="A43" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D43" s="16">
-        <v>3.1</v>
-      </c>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="L43" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="M43" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="N43" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="O43" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="P43" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q43" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="R43" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" s="10" customFormat="1" ht="89.25">
-      <c r="A44" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D44" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="L44" s="1"/>
-      <c r="M44" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="N44" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="O44" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="P44" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q44" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R44" s="1"/>
-    </row>
-    <row r="45" spans="1:18" s="10" customFormat="1" ht="114.75" customHeight="1">
-      <c r="A45" s="11"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
-      <c r="I45" s="11"/>
-      <c r="J45" s="11"/>
-      <c r="K45" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="L45" s="33"/>
-      <c r="M45" s="33"/>
-      <c r="N45" s="33"/>
-      <c r="O45" s="33"/>
-      <c r="P45" s="33"/>
-      <c r="Q45" s="33"/>
-      <c r="R45" s="34"/>
+      <c r="L63" s="33"/>
+      <c r="M63" s="33"/>
+      <c r="N63" s="33"/>
+      <c r="O63" s="33"/>
+      <c r="P63" s="33"/>
+      <c r="Q63" s="33"/>
+      <c r="R63" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="K2:R2"/>
-    <mergeCell ref="K45:R45"/>
+    <mergeCell ref="K63:R63"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="44" orientation="landscape" copies="3" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="32" max="13" man="1"/>
+    <brk id="50" max="13" man="1"/>
   </rowBreaks>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>

</xml_diff>

<commit_message>
Updates towards an editor for interventiebeleid
</commit_message>
<xml_diff>
--- a/Blik/Interventiebeleid tabak.xlsx
+++ b/Blik/Interventiebeleid tabak.xlsx
@@ -903,9 +903,6 @@
     <t>rechtsgrond</t>
   </si>
   <si>
-    <t>Rechtsgrond</t>
-  </si>
-  <si>
     <t>[Rechtspersoonsoort,]</t>
   </si>
   <si>
@@ -988,6 +985,9 @@
   </si>
   <si>
     <t>bepaling</t>
+  </si>
+  <si>
+    <t>RechtsGrond</t>
   </si>
 </sst>
 </file>
@@ -1573,7 +1573,7 @@
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="75" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -1706,7 +1706,7 @@
         <v>162</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>267</v>
@@ -1764,10 +1764,10 @@
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15" t="s">
+        <v>296</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>268</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>269</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>174</v>
@@ -1823,7 +1823,7 @@
         <v>248</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>172</v>
@@ -1855,7 +1855,7 @@
         <v>249</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>163</v>
@@ -1903,7 +1903,7 @@
         <v>250</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>163</v>
@@ -1956,7 +1956,7 @@
         <v>251</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>163</v>
@@ -2005,7 +2005,7 @@
         <v>251</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>189</v>
@@ -2044,7 +2044,7 @@
         <v>252</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -2089,7 +2089,7 @@
         <v>253</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -2134,7 +2134,7 @@
         <v>265</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -2179,7 +2179,7 @@
         <v>254</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -2222,7 +2222,7 @@
         <v>255</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -2267,7 +2267,7 @@
         <v>256</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -2312,7 +2312,7 @@
         <v>257</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -2355,7 +2355,7 @@
         <v>258</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -2398,7 +2398,7 @@
         <v>259</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -2445,7 +2445,7 @@
         <v>260</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -2488,7 +2488,7 @@
         <v>261</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -2531,7 +2531,7 @@
         <v>262</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -2576,7 +2576,7 @@
         <v>263</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -2621,7 +2621,7 @@
         <v>263</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -2666,7 +2666,7 @@
         <v>263</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
@@ -2711,7 +2711,7 @@
         <v>263</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -2754,7 +2754,7 @@
         <v>207</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F27" s="16" t="s">
         <v>208</v>
@@ -2807,7 +2807,7 @@
         <v>207</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F28" s="16" t="s">
         <v>208</v>
@@ -2862,7 +2862,7 @@
         <v>207</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F29" s="16" t="s">
         <v>208</v>
@@ -2917,7 +2917,7 @@
         <v>214</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F30" s="16" t="s">
         <v>219</v>
@@ -2970,7 +2970,7 @@
         <v>214</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F31" s="16" t="s">
         <v>219</v>
@@ -3025,7 +3025,7 @@
         <v>214</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F32" s="16" t="s">
         <v>219</v>
@@ -3080,7 +3080,7 @@
         <v>222</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F33" s="16" t="s">
         <v>221</v>
@@ -3133,7 +3133,7 @@
         <v>222</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F34" s="16" t="s">
         <v>221</v>
@@ -3188,7 +3188,7 @@
         <v>222</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F35" s="16" t="s">
         <v>221</v>
@@ -3243,7 +3243,7 @@
         <v>227</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F36" s="16" t="s">
         <v>219</v>
@@ -3296,7 +3296,7 @@
         <v>227</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F37" s="16" t="s">
         <v>219</v>
@@ -3351,7 +3351,7 @@
         <v>227</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F38" s="16" t="s">
         <v>219</v>
@@ -3406,7 +3406,7 @@
         <v>232</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F39" s="16" t="s">
         <v>236</v>
@@ -3459,7 +3459,7 @@
         <v>232</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F40" s="16" t="s">
         <v>236</v>
@@ -3514,7 +3514,7 @@
         <v>232</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F41" s="16" t="s">
         <v>236</v>
@@ -3569,7 +3569,7 @@
         <v>238</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F42" s="16" t="s">
         <v>242</v>
@@ -3679,7 +3679,7 @@
         <v>238</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F44" s="16" t="s">
         <v>242</v>
@@ -3734,7 +3734,7 @@
         <v>238</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F45" s="16" t="s">
         <v>242</v>
@@ -3789,7 +3789,7 @@
         <v>244</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F46" s="16" t="s">
         <v>242</v>
@@ -3842,7 +3842,7 @@
         <v>244</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F47" s="16" t="s">
         <v>242</v>
@@ -3897,7 +3897,7 @@
         <v>244</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F48" s="16" t="s">
         <v>242</v>
@@ -4382,7 +4382,7 @@
         <v>248</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
@@ -4431,7 +4431,7 @@
         <v>266</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
@@ -4480,7 +4480,7 @@
         <v>248</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
@@ -4529,7 +4529,7 @@
         <v>264</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>

</xml_diff>

<commit_message>
updates for analyzing issue #355
</commit_message>
<xml_diff>
--- a/Blik/Interventiebeleid tabak.xlsx
+++ b/Blik/Interventiebeleid tabak.xlsx
@@ -1445,15 +1445,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1503,6 +1494,15 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1572,7 +1572,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>19</xdr:col>
-          <xdr:colOff>1473200</xdr:colOff>
+          <xdr:colOff>1476375</xdr:colOff>
           <xdr:row>19</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -1894,9 +1894,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T65"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="75" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A26" sqref="A26:A27"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="I1" zoomScale="75" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -1921,13 +1921,13 @@
   <sheetData>
     <row r="1" spans="1:20" s="9" customFormat="1" ht="66" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="46" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="28"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="47"/>
       <c r="G1" s="23"/>
       <c r="H1" s="23"/>
       <c r="I1" s="23"/>
@@ -1950,10 +1950,10 @@
         <v>7</v>
       </c>
       <c r="B2" s="5"/>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="29"/>
+      <c r="D2" s="48"/>
       <c r="E2" s="25"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -1963,15 +1963,15 @@
       <c r="K2" s="2"/>
       <c r="L2" s="26"/>
       <c r="M2" s="26"/>
-      <c r="N2" s="29" t="s">
+      <c r="N2" s="48" t="s">
         <v>337</v>
       </c>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
-      <c r="T2" s="29"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="Q2" s="48"/>
+      <c r="R2" s="48"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="48"/>
     </row>
     <row r="3" spans="1:20" s="10" customFormat="1" ht="50.25" customHeight="1">
       <c r="A3" s="3" t="s">
@@ -1997,13 +1997,13 @@
       <c r="K3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="41" t="s">
+      <c r="L3" s="38" t="s">
         <v>291</v>
       </c>
-      <c r="M3" s="41" t="s">
+      <c r="M3" s="38" t="s">
         <v>291</v>
       </c>
-      <c r="N3" s="36" t="s">
+      <c r="N3" s="33" t="s">
         <v>274</v>
       </c>
       <c r="O3" s="3" t="s">
@@ -2057,10 +2057,10 @@
       <c r="K4" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="L4" s="42" t="s">
+      <c r="L4" s="39" t="s">
         <v>347</v>
       </c>
-      <c r="M4" s="42" t="s">
+      <c r="M4" s="39" t="s">
         <v>346</v>
       </c>
       <c r="N4" s="3" t="s">
@@ -2159,7 +2159,7 @@
       <c r="E6" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="F6" s="40" t="s">
+      <c r="F6" s="37" t="s">
         <v>289</v>
       </c>
       <c r="G6" s="7" t="s">
@@ -2174,7 +2174,7 @@
       <c r="K6" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="N6" s="34" t="s">
+      <c r="N6" s="31" t="s">
         <v>288</v>
       </c>
       <c r="S6" s="7" t="s">
@@ -2209,7 +2209,7 @@
       <c r="I7" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="N7" s="34" t="s">
+      <c r="N7" s="31" t="s">
         <v>275</v>
       </c>
       <c r="O7" s="1" t="s">
@@ -2257,7 +2257,7 @@
       <c r="K8" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="N8" s="34" t="s">
+      <c r="N8" s="31" t="s">
         <v>276</v>
       </c>
       <c r="O8" s="7" t="s">
@@ -2308,7 +2308,7 @@
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
-      <c r="N9" s="39" t="s">
+      <c r="N9" s="36" t="s">
         <v>287</v>
       </c>
       <c r="O9" s="1" t="s">
@@ -2356,7 +2356,7 @@
       </c>
       <c r="L10" s="24"/>
       <c r="M10" s="24"/>
-      <c r="N10" s="34"/>
+      <c r="N10" s="31"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
@@ -2380,7 +2380,7 @@
       <c r="E11" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="F11" s="40" t="s">
+      <c r="F11" s="37" t="s">
         <v>289</v>
       </c>
       <c r="G11" s="1"/>
@@ -2426,7 +2426,7 @@
       <c r="E12" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="F12" s="40" t="s">
+      <c r="F12" s="37" t="s">
         <v>289</v>
       </c>
       <c r="G12" s="1" t="s">
@@ -2474,7 +2474,7 @@
       <c r="E13" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="F13" s="40" t="s">
+      <c r="F13" s="37" t="s">
         <v>289</v>
       </c>
       <c r="G13" s="1"/>
@@ -2520,7 +2520,7 @@
       <c r="E14" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="F14" s="40" t="s">
+      <c r="F14" s="37" t="s">
         <v>289</v>
       </c>
       <c r="G14" s="1"/>
@@ -2564,7 +2564,7 @@
       <c r="E15" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="F15" s="40" t="s">
+      <c r="F15" s="37" t="s">
         <v>289</v>
       </c>
       <c r="G15" s="1"/>
@@ -2610,7 +2610,7 @@
       <c r="E16" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="F16" s="40" t="s">
+      <c r="F16" s="37" t="s">
         <v>289</v>
       </c>
       <c r="G16" s="1"/>
@@ -2656,7 +2656,7 @@
       <c r="E17" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="F17" s="40" t="s">
+      <c r="F17" s="37" t="s">
         <v>289</v>
       </c>
       <c r="G17" s="1"/>
@@ -2700,29 +2700,29 @@
       <c r="E18" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="F18" s="40" t="s">
+      <c r="F18" s="37" t="s">
         <v>289</v>
       </c>
-      <c r="G18" s="40" t="s">
+      <c r="G18" s="37" t="s">
         <v>138</v>
       </c>
-      <c r="H18" s="40" t="s">
+      <c r="H18" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="I18" s="40" t="s">
+      <c r="I18" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="J18" s="40" t="s">
+      <c r="J18" s="37" t="s">
         <v>299</v>
       </c>
       <c r="K18" s="1"/>
-      <c r="L18" s="43" t="s">
+      <c r="L18" s="40" t="s">
         <v>292</v>
       </c>
-      <c r="M18" s="40" t="s">
+      <c r="M18" s="37" t="s">
         <v>343</v>
       </c>
-      <c r="N18" s="34" t="s">
+      <c r="N18" s="31" t="s">
         <v>290</v>
       </c>
       <c r="O18" s="1"/>
@@ -2743,87 +2743,87 @@
     <row r="19" spans="1:20" s="10" customFormat="1" ht="201" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="7"/>
-      <c r="C19" s="40" t="s">
+      <c r="C19" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="44" t="s">
+      <c r="D19" s="41" t="s">
         <v>220</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="F19" s="40" t="s">
+      <c r="F19" s="37" t="s">
         <v>289</v>
       </c>
-      <c r="G19" s="40" t="s">
+      <c r="G19" s="37" t="s">
         <v>138</v>
       </c>
-      <c r="H19" s="40" t="s">
+      <c r="H19" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="I19" s="40" t="s">
+      <c r="I19" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="J19" s="40" t="s">
+      <c r="J19" s="37" t="s">
         <v>294</v>
       </c>
-      <c r="K19" s="40"/>
-      <c r="L19" s="43" t="s">
+      <c r="K19" s="37"/>
+      <c r="L19" s="40" t="s">
         <v>292</v>
       </c>
-      <c r="M19" s="40" t="s">
+      <c r="M19" s="37" t="s">
         <v>293</v>
       </c>
-      <c r="N19" s="40" t="s">
+      <c r="N19" s="37" t="s">
         <v>277</v>
       </c>
-      <c r="O19" s="40"/>
-      <c r="P19" s="40" t="s">
+      <c r="O19" s="37"/>
+      <c r="P19" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="Q19" s="40" t="s">
+      <c r="Q19" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="R19" s="40" t="s">
+      <c r="R19" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="S19" s="40" t="s">
+      <c r="S19" s="37" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:20" s="10" customFormat="1" ht="201" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="7"/>
-      <c r="C20" s="40" t="s">
+      <c r="C20" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="44" t="s">
+      <c r="D20" s="41" t="s">
         <v>295</v>
       </c>
-      <c r="E20" s="47" t="s">
+      <c r="E20" s="44" t="s">
         <v>342</v>
       </c>
-      <c r="F20" s="40" t="s">
+      <c r="F20" s="37" t="s">
         <v>289</v>
       </c>
-      <c r="G20" s="40" t="s">
+      <c r="G20" s="37" t="s">
         <v>142</v>
       </c>
-      <c r="H20" s="40" t="s">
+      <c r="H20" s="37" t="s">
         <v>296</v>
       </c>
-      <c r="I20" s="40"/>
-      <c r="J20" s="40"/>
-      <c r="K20" s="40" t="s">
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="37" t="s">
         <v>297</v>
       </c>
-      <c r="L20" s="43" t="s">
+      <c r="L20" s="40" t="s">
         <v>292</v>
       </c>
-      <c r="M20" s="40" t="s">
+      <c r="M20" s="37" t="s">
         <v>343</v>
       </c>
-      <c r="N20" s="34"/>
+      <c r="N20" s="31"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
@@ -2847,27 +2847,27 @@
       <c r="E21" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="F21" s="40" t="s">
+      <c r="F21" s="37" t="s">
         <v>289</v>
       </c>
-      <c r="G21" s="40" t="s">
+      <c r="G21" s="37" t="s">
         <v>142</v>
       </c>
-      <c r="H21" s="40" t="s">
+      <c r="H21" s="37" t="s">
         <v>300</v>
       </c>
-      <c r="I21" s="40" t="s">
+      <c r="I21" s="37" t="s">
         <v>301</v>
       </c>
-      <c r="J21" s="40"/>
-      <c r="K21" s="40" t="s">
+      <c r="J21" s="37"/>
+      <c r="K21" s="37" t="s">
         <v>302</v>
       </c>
-      <c r="L21" s="40"/>
-      <c r="M21" s="40" t="s">
+      <c r="L21" s="37"/>
+      <c r="M21" s="37" t="s">
         <v>343</v>
       </c>
-      <c r="N21" s="40" t="s">
+      <c r="N21" s="37" t="s">
         <v>278</v>
       </c>
       <c r="O21" s="1" t="s">
@@ -2905,29 +2905,29 @@
       <c r="E22" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="F22" s="40" t="s">
+      <c r="F22" s="37" t="s">
         <v>289</v>
       </c>
-      <c r="G22" s="40" t="s">
+      <c r="G22" s="37" t="s">
         <v>138</v>
       </c>
-      <c r="H22" s="40" t="s">
+      <c r="H22" s="37" t="s">
         <v>303</v>
       </c>
-      <c r="I22" s="40" t="s">
+      <c r="I22" s="37" t="s">
         <v>304</v>
       </c>
-      <c r="J22" s="40" t="s">
+      <c r="J22" s="37" t="s">
         <v>305</v>
       </c>
-      <c r="K22" s="40"/>
-      <c r="L22" s="40" t="s">
+      <c r="K22" s="37"/>
+      <c r="L22" s="37" t="s">
         <v>313</v>
       </c>
-      <c r="M22" s="40" t="s">
+      <c r="M22" s="37" t="s">
         <v>343</v>
       </c>
-      <c r="N22" s="40" t="s">
+      <c r="N22" s="37" t="s">
         <v>279</v>
       </c>
       <c r="O22" s="1"/>
@@ -2961,31 +2961,31 @@
       <c r="E23" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="F23" s="40" t="s">
+      <c r="F23" s="37" t="s">
         <v>289</v>
       </c>
-      <c r="G23" s="40" t="s">
+      <c r="G23" s="37" t="s">
         <v>138</v>
       </c>
-      <c r="H23" s="40" t="s">
+      <c r="H23" s="37" t="s">
         <v>306</v>
       </c>
-      <c r="I23" s="40" t="s">
+      <c r="I23" s="37" t="s">
         <v>307</v>
       </c>
-      <c r="J23" s="40" t="s">
+      <c r="J23" s="37" t="s">
         <v>345</v>
       </c>
-      <c r="K23" s="40" t="s">
+      <c r="K23" s="37" t="s">
         <v>308</v>
       </c>
-      <c r="L23" s="40" t="s">
+      <c r="L23" s="37" t="s">
         <v>314</v>
       </c>
-      <c r="M23" s="40" t="s">
+      <c r="M23" s="37" t="s">
         <v>343</v>
       </c>
-      <c r="N23" s="40" t="s">
+      <c r="N23" s="37" t="s">
         <v>280</v>
       </c>
       <c r="O23" s="1"/>
@@ -3019,29 +3019,29 @@
       <c r="E24" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="F24" s="40" t="s">
+      <c r="F24" s="37" t="s">
         <v>289</v>
       </c>
-      <c r="G24" s="40" t="s">
+      <c r="G24" s="37" t="s">
         <v>138</v>
       </c>
-      <c r="H24" s="40" t="s">
+      <c r="H24" s="37" t="s">
         <v>309</v>
       </c>
-      <c r="I24" s="40" t="s">
+      <c r="I24" s="37" t="s">
         <v>307</v>
       </c>
-      <c r="J24" s="40"/>
-      <c r="K24" s="40" t="s">
+      <c r="J24" s="37"/>
+      <c r="K24" s="37" t="s">
         <v>310</v>
       </c>
-      <c r="L24" s="40" t="s">
+      <c r="L24" s="37" t="s">
         <v>315</v>
       </c>
-      <c r="M24" s="40" t="s">
+      <c r="M24" s="37" t="s">
         <v>343</v>
       </c>
-      <c r="N24" s="40" t="s">
+      <c r="N24" s="37" t="s">
         <v>281</v>
       </c>
       <c r="O24" s="1" t="s">
@@ -3077,31 +3077,31 @@
       <c r="E25" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="F25" s="40" t="s">
+      <c r="F25" s="37" t="s">
         <v>289</v>
       </c>
-      <c r="G25" s="40" t="s">
+      <c r="G25" s="37" t="s">
         <v>298</v>
       </c>
-      <c r="H25" s="40" t="s">
+      <c r="H25" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="I25" s="40" t="s">
+      <c r="I25" s="37" t="s">
         <v>311</v>
       </c>
-      <c r="J25" s="40" t="s">
+      <c r="J25" s="37" t="s">
         <v>345</v>
       </c>
-      <c r="K25" s="40" t="s">
+      <c r="K25" s="37" t="s">
         <v>312</v>
       </c>
-      <c r="L25" s="45" t="s">
+      <c r="L25" s="42" t="s">
         <v>344</v>
       </c>
-      <c r="M25" s="40" t="s">
+      <c r="M25" s="37" t="s">
         <v>343</v>
       </c>
-      <c r="N25" s="40"/>
+      <c r="N25" s="37"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1" t="s">
         <v>66</v>
@@ -3122,96 +3122,96 @@
     <row r="26" spans="1:20" s="10" customFormat="1" ht="59.25" customHeight="1">
       <c r="A26" s="1"/>
       <c r="B26" s="7"/>
-      <c r="C26" s="40" t="s">
+      <c r="C26" s="37" t="s">
         <v>316</v>
       </c>
-      <c r="D26" s="44" t="s">
+      <c r="D26" s="41" t="s">
         <v>317</v>
       </c>
-      <c r="E26" s="48" t="s">
+      <c r="E26" s="45" t="s">
         <v>338</v>
       </c>
-      <c r="F26" s="40" t="s">
+      <c r="F26" s="37" t="s">
         <v>289</v>
       </c>
-      <c r="G26" s="40" t="s">
+      <c r="G26" s="37" t="s">
         <v>138</v>
       </c>
-      <c r="H26" s="40" t="s">
+      <c r="H26" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="I26" s="40" t="s">
+      <c r="I26" s="37" t="s">
         <v>318</v>
       </c>
-      <c r="J26" s="40" t="s">
+      <c r="J26" s="37" t="s">
         <v>345</v>
       </c>
-      <c r="K26" s="40"/>
-      <c r="L26" s="45" t="s">
+      <c r="K26" s="37"/>
+      <c r="L26" s="42" t="s">
         <v>344</v>
       </c>
-      <c r="M26" s="40" t="s">
+      <c r="M26" s="37" t="s">
         <v>343</v>
       </c>
-      <c r="N26" s="40" t="s">
+      <c r="N26" s="37" t="s">
         <v>326</v>
       </c>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
-      <c r="Q26" s="40"/>
-      <c r="R26" s="40"/>
-      <c r="S26" s="40"/>
-      <c r="T26" s="46"/>
+      <c r="Q26" s="37"/>
+      <c r="R26" s="37"/>
+      <c r="S26" s="37"/>
+      <c r="T26" s="43"/>
     </row>
     <row r="27" spans="1:20" s="10" customFormat="1" ht="59.25" customHeight="1">
       <c r="A27" s="1"/>
       <c r="B27" s="7"/>
-      <c r="C27" s="40" t="s">
+      <c r="C27" s="37" t="s">
         <v>316</v>
       </c>
-      <c r="D27" s="44" t="s">
+      <c r="D27" s="41" t="s">
         <v>319</v>
       </c>
-      <c r="E27" s="48" t="s">
+      <c r="E27" s="45" t="s">
         <v>339</v>
       </c>
-      <c r="F27" s="40" t="s">
+      <c r="F27" s="37" t="s">
         <v>289</v>
       </c>
-      <c r="G27" s="40"/>
-      <c r="H27" s="40" t="s">
+      <c r="G27" s="37"/>
+      <c r="H27" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="I27" s="40" t="s">
+      <c r="I27" s="37" t="s">
         <v>320</v>
       </c>
-      <c r="J27" s="40"/>
-      <c r="K27" s="40" t="s">
+      <c r="J27" s="37"/>
+      <c r="K27" s="37" t="s">
         <v>327</v>
       </c>
-      <c r="L27" s="40" t="s">
+      <c r="L27" s="37" t="s">
         <v>328</v>
       </c>
-      <c r="M27" s="40" t="s">
+      <c r="M27" s="37" t="s">
         <v>343</v>
       </c>
-      <c r="N27" s="40" t="s">
+      <c r="N27" s="37" t="s">
         <v>282</v>
       </c>
       <c r="O27" s="1"/>
       <c r="P27" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="Q27" s="40" t="s">
+      <c r="Q27" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="R27" s="40" t="s">
+      <c r="R27" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="S27" s="40" t="s">
+      <c r="S27" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="T27" s="46" t="s">
+      <c r="T27" s="43" t="s">
         <v>53</v>
       </c>
     </row>
@@ -3222,52 +3222,52 @@
       <c r="B28" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="40" t="s">
+      <c r="C28" s="37" t="s">
         <v>316</v>
       </c>
-      <c r="D28" s="44" t="s">
+      <c r="D28" s="41" t="s">
         <v>319</v>
       </c>
-      <c r="E28" s="48" t="s">
+      <c r="E28" s="45" t="s">
         <v>339</v>
       </c>
-      <c r="F28" s="40" t="s">
+      <c r="F28" s="37" t="s">
         <v>289</v>
       </c>
-      <c r="G28" s="40"/>
-      <c r="H28" s="40" t="s">
+      <c r="G28" s="37"/>
+      <c r="H28" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="I28" s="40" t="s">
+      <c r="I28" s="37" t="s">
         <v>320</v>
       </c>
-      <c r="J28" s="40"/>
-      <c r="K28" s="40" t="s">
+      <c r="J28" s="37"/>
+      <c r="K28" s="37" t="s">
         <v>327</v>
       </c>
-      <c r="L28" s="40" t="s">
+      <c r="L28" s="37" t="s">
         <v>328</v>
       </c>
-      <c r="M28" s="40" t="s">
+      <c r="M28" s="37" t="s">
         <v>343</v>
       </c>
-      <c r="N28" s="40" t="s">
+      <c r="N28" s="37" t="s">
         <v>283</v>
       </c>
       <c r="O28" s="1"/>
       <c r="P28" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="Q28" s="40" t="s">
+      <c r="Q28" s="37" t="s">
         <v>332</v>
       </c>
-      <c r="R28" s="40" t="s">
+      <c r="R28" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="S28" s="40" t="s">
+      <c r="S28" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="T28" s="46" t="s">
+      <c r="T28" s="43" t="s">
         <v>333</v>
       </c>
     </row>
@@ -3278,54 +3278,54 @@
       <c r="B29" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="40" t="s">
+      <c r="C29" s="37" t="s">
         <v>316</v>
       </c>
-      <c r="D29" s="44" t="s">
+      <c r="D29" s="41" t="s">
         <v>321</v>
       </c>
-      <c r="E29" s="47" t="s">
+      <c r="E29" s="44" t="s">
         <v>340</v>
       </c>
-      <c r="F29" s="40" t="s">
+      <c r="F29" s="37" t="s">
         <v>289</v>
       </c>
-      <c r="G29" s="40" t="s">
+      <c r="G29" s="37" t="s">
         <v>322</v>
       </c>
-      <c r="H29" s="40" t="s">
+      <c r="H29" s="37" t="s">
         <v>323</v>
       </c>
-      <c r="I29" s="40" t="s">
+      <c r="I29" s="37" t="s">
         <v>324</v>
       </c>
-      <c r="J29" s="40"/>
-      <c r="K29" s="40" t="s">
+      <c r="J29" s="37"/>
+      <c r="K29" s="37" t="s">
         <v>329</v>
       </c>
-      <c r="L29" s="40" t="s">
+      <c r="L29" s="37" t="s">
         <v>330</v>
       </c>
-      <c r="M29" s="40" t="s">
+      <c r="M29" s="37" t="s">
         <v>343</v>
       </c>
-      <c r="N29" s="40" t="s">
+      <c r="N29" s="37" t="s">
         <v>284</v>
       </c>
       <c r="O29" s="1"/>
       <c r="P29" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="Q29" s="40" t="s">
+      <c r="Q29" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="R29" s="40" t="s">
+      <c r="R29" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="S29" s="40" t="s">
+      <c r="S29" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="T29" s="46" t="s">
+      <c r="T29" s="43" t="s">
         <v>53</v>
       </c>
     </row>
@@ -3336,54 +3336,54 @@
       <c r="B30" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C30" s="40" t="s">
+      <c r="C30" s="37" t="s">
         <v>316</v>
       </c>
-      <c r="D30" s="44" t="s">
+      <c r="D30" s="41" t="s">
         <v>325</v>
       </c>
-      <c r="E30" s="47" t="s">
+      <c r="E30" s="44" t="s">
         <v>341</v>
       </c>
-      <c r="F30" s="40" t="s">
+      <c r="F30" s="37" t="s">
         <v>289</v>
       </c>
-      <c r="G30" s="40" t="s">
+      <c r="G30" s="37" t="s">
         <v>322</v>
       </c>
-      <c r="H30" s="40" t="s">
+      <c r="H30" s="37" t="s">
         <v>323</v>
       </c>
-      <c r="I30" s="40" t="s">
+      <c r="I30" s="37" t="s">
         <v>324</v>
       </c>
-      <c r="J30" s="40"/>
-      <c r="K30" s="40" t="s">
+      <c r="J30" s="37"/>
+      <c r="K30" s="37" t="s">
         <v>331</v>
       </c>
-      <c r="L30" s="40" t="s">
+      <c r="L30" s="37" t="s">
         <v>330</v>
       </c>
-      <c r="M30" s="40" t="s">
+      <c r="M30" s="37" t="s">
         <v>343</v>
       </c>
-      <c r="N30" s="40" t="s">
+      <c r="N30" s="37" t="s">
         <v>285</v>
       </c>
       <c r="O30" s="1"/>
       <c r="P30" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="Q30" s="40" t="s">
+      <c r="Q30" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="R30" s="40" t="s">
+      <c r="R30" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="S30" s="40" t="s">
+      <c r="S30" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="T30" s="46" t="s">
+      <c r="T30" s="43" t="s">
         <v>53</v>
       </c>
     </row>
@@ -3419,7 +3419,7 @@
       </c>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
-      <c r="N31" s="34" t="s">
+      <c r="N31" s="31" t="s">
         <v>282</v>
       </c>
       <c r="O31" s="1" t="s">
@@ -3471,7 +3471,7 @@
       </c>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
-      <c r="N32" s="34" t="s">
+      <c r="N32" s="31" t="s">
         <v>283</v>
       </c>
       <c r="O32" s="1" t="s">
@@ -3525,7 +3525,7 @@
       </c>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
-      <c r="N33" s="34" t="s">
+      <c r="N33" s="31" t="s">
         <v>284</v>
       </c>
       <c r="O33" s="1" t="s">
@@ -3579,7 +3579,7 @@
       </c>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
-      <c r="N34" s="34" t="s">
+      <c r="N34" s="31" t="s">
         <v>285</v>
       </c>
       <c r="O34" s="1" t="s">
@@ -3631,7 +3631,7 @@
       </c>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
-      <c r="N35" s="37"/>
+      <c r="N35" s="34"/>
       <c r="O35" s="1" t="s">
         <v>109</v>
       </c>
@@ -3683,7 +3683,7 @@
       </c>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
-      <c r="N36" s="38"/>
+      <c r="N36" s="35"/>
       <c r="O36" s="1" t="s">
         <v>106</v>
       </c>
@@ -3735,7 +3735,7 @@
       </c>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
-      <c r="N37" s="38"/>
+      <c r="N37" s="35"/>
       <c r="O37" s="1" t="s">
         <v>95</v>
       </c>
@@ -3785,7 +3785,7 @@
       </c>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
-      <c r="N38" s="38"/>
+      <c r="N38" s="35"/>
       <c r="O38" s="1" t="s">
         <v>109</v>
       </c>
@@ -3837,7 +3837,7 @@
       </c>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
-      <c r="N39" s="34"/>
+      <c r="N39" s="31"/>
       <c r="O39" s="1" t="s">
         <v>106</v>
       </c>
@@ -3889,7 +3889,7 @@
       </c>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
-      <c r="N40" s="34"/>
+      <c r="N40" s="31"/>
       <c r="O40" s="1" t="s">
         <v>95</v>
       </c>
@@ -3939,7 +3939,7 @@
       </c>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
-      <c r="N41" s="34"/>
+      <c r="N41" s="31"/>
       <c r="O41" s="1" t="s">
         <v>109</v>
       </c>
@@ -3991,7 +3991,7 @@
       </c>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
-      <c r="N42" s="32"/>
+      <c r="N42" s="29"/>
       <c r="O42" s="1" t="s">
         <v>106</v>
       </c>
@@ -4041,11 +4041,11 @@
       <c r="K43" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="L43" s="40" t="s">
+      <c r="L43" s="37" t="s">
         <v>334</v>
       </c>
       <c r="M43" s="1"/>
-      <c r="N43" s="40" t="s">
+      <c r="N43" s="37" t="s">
         <v>286</v>
       </c>
       <c r="O43" s="1" t="s">
@@ -4095,11 +4095,11 @@
       <c r="K44" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="L44" s="40" t="s">
+      <c r="L44" s="37" t="s">
         <v>335</v>
       </c>
       <c r="M44" s="1"/>
-      <c r="N44" s="40" t="s">
+      <c r="N44" s="37" t="s">
         <v>286</v>
       </c>
       <c r="O44" s="1" t="s">
@@ -4151,11 +4151,11 @@
       <c r="K45" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="L45" s="40" t="s">
+      <c r="L45" s="37" t="s">
         <v>336</v>
       </c>
       <c r="M45" s="1"/>
-      <c r="N45" s="40" t="s">
+      <c r="N45" s="37" t="s">
         <v>286</v>
       </c>
       <c r="O45" s="1" t="s">
@@ -4209,7 +4209,7 @@
       </c>
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
-      <c r="N46" s="32"/>
+      <c r="N46" s="29"/>
       <c r="O46" s="1" t="s">
         <v>95</v>
       </c>
@@ -4259,7 +4259,7 @@
       </c>
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
-      <c r="N47" s="32"/>
+      <c r="N47" s="29"/>
       <c r="O47" s="1" t="s">
         <v>109</v>
       </c>
@@ -4311,7 +4311,7 @@
       </c>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
-      <c r="N48" s="32"/>
+      <c r="N48" s="29"/>
       <c r="O48" s="1" t="s">
         <v>106</v>
       </c>
@@ -4363,7 +4363,7 @@
       </c>
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
-      <c r="N49" s="32"/>
+      <c r="N49" s="29"/>
       <c r="O49" s="1" t="s">
         <v>95</v>
       </c>
@@ -4413,7 +4413,7 @@
       </c>
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
-      <c r="N50" s="32"/>
+      <c r="N50" s="29"/>
       <c r="O50" s="1" t="s">
         <v>109</v>
       </c>
@@ -4465,7 +4465,7 @@
       </c>
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
-      <c r="N51" s="34" t="s">
+      <c r="N51" s="31" t="s">
         <v>286</v>
       </c>
       <c r="O51" s="1" t="s">
@@ -4509,7 +4509,7 @@
       </c>
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
-      <c r="N52" s="34" t="s">
+      <c r="N52" s="31" t="s">
         <v>286</v>
       </c>
       <c r="O52" s="1" t="s">
@@ -4551,7 +4551,7 @@
       </c>
       <c r="L53" s="17"/>
       <c r="M53" s="17"/>
-      <c r="N53" s="34" t="s">
+      <c r="N53" s="31" t="s">
         <v>286</v>
       </c>
       <c r="O53" s="17" t="s">
@@ -4595,7 +4595,7 @@
       </c>
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
-      <c r="N54" s="32"/>
+      <c r="N54" s="29"/>
       <c r="O54" s="1" t="s">
         <v>96</v>
       </c>
@@ -4635,7 +4635,7 @@
       </c>
       <c r="L55" s="1"/>
       <c r="M55" s="1"/>
-      <c r="N55" s="32"/>
+      <c r="N55" s="29"/>
       <c r="O55" s="1" t="s">
         <v>105</v>
       </c>
@@ -4675,7 +4675,7 @@
       </c>
       <c r="L56" s="17"/>
       <c r="M56" s="17"/>
-      <c r="N56" s="32"/>
+      <c r="N56" s="29"/>
       <c r="O56" s="17"/>
       <c r="P56" s="17" t="s">
         <v>111</v>
@@ -4715,7 +4715,7 @@
       </c>
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
-      <c r="N57" s="32"/>
+      <c r="N57" s="29"/>
       <c r="O57" s="1"/>
       <c r="P57" s="1" t="s">
         <v>67</v>
@@ -4751,7 +4751,7 @@
       </c>
       <c r="L58" s="17"/>
       <c r="M58" s="17"/>
-      <c r="N58" s="32"/>
+      <c r="N58" s="29"/>
       <c r="O58" s="17"/>
       <c r="P58" s="17" t="s">
         <v>67</v>
@@ -4791,7 +4791,7 @@
       </c>
       <c r="L59" s="1"/>
       <c r="M59" s="1"/>
-      <c r="N59" s="32"/>
+      <c r="N59" s="29"/>
       <c r="O59" s="1"/>
       <c r="P59" s="1" t="s">
         <v>66</v>
@@ -4829,7 +4829,7 @@
       </c>
       <c r="L60" s="1"/>
       <c r="M60" s="1"/>
-      <c r="N60" s="32"/>
+      <c r="N60" s="29"/>
       <c r="O60" s="1"/>
       <c r="P60" s="1" t="s">
         <v>67</v>
@@ -4857,7 +4857,7 @@
       </c>
       <c r="D61" s="14"/>
       <c r="E61" s="14"/>
-      <c r="F61" s="40" t="s">
+      <c r="F61" s="37" t="s">
         <v>289</v>
       </c>
       <c r="G61" s="1"/>
@@ -4871,7 +4871,7 @@
       </c>
       <c r="L61" s="1"/>
       <c r="M61" s="1"/>
-      <c r="N61" s="33"/>
+      <c r="N61" s="30"/>
       <c r="O61" s="8" t="s">
         <v>56</v>
       </c>
@@ -4907,7 +4907,7 @@
       <c r="E62" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="F62" s="40" t="s">
+      <c r="F62" s="37" t="s">
         <v>289</v>
       </c>
       <c r="G62" s="1"/>
@@ -4919,7 +4919,7 @@
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
       <c r="M62" s="1"/>
-      <c r="N62" s="32"/>
+      <c r="N62" s="29"/>
       <c r="O62" s="1" t="s">
         <v>59</v>
       </c>
@@ -4955,7 +4955,7 @@
       <c r="E63" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="F63" s="40" t="s">
+      <c r="F63" s="37" t="s">
         <v>289</v>
       </c>
       <c r="G63" s="1"/>
@@ -4967,7 +4967,7 @@
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
       <c r="M63" s="1"/>
-      <c r="N63" s="32"/>
+      <c r="N63" s="29"/>
       <c r="O63" s="1" t="s">
         <v>59</v>
       </c>
@@ -5003,7 +5003,7 @@
       <c r="E64" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="F64" s="40" t="s">
+      <c r="F64" s="37" t="s">
         <v>289</v>
       </c>
       <c r="G64" s="1"/>
@@ -5015,7 +5015,7 @@
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
       <c r="M64" s="1"/>
-      <c r="N64" s="35"/>
+      <c r="N64" s="32"/>
       <c r="O64" s="1" t="s">
         <v>60</v>
       </c>
@@ -5051,7 +5051,7 @@
       <c r="E65" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="F65" s="40" t="s">
+      <c r="F65" s="37" t="s">
         <v>289</v>
       </c>
       <c r="G65" s="1"/>
@@ -5063,7 +5063,7 @@
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
       <c r="M65" s="1"/>
-      <c r="N65" s="35"/>
+      <c r="N65" s="32"/>
       <c r="O65" s="1"/>
       <c r="P65" s="1" t="s">
         <v>66</v>
@@ -5219,57 +5219,57 @@
   <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="27" t="s">
         <v>262</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="27" t="s">
         <v>263</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="28" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="27" t="s">
         <v>265</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="27" t="s">
         <v>157</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="28" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="28" t="s">
         <v>267</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="28" t="s">
         <v>268</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="28" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="28" t="s">
         <v>270</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="28" t="s">
         <v>271</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="28" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="28" t="s">
         <v>272</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="28" t="s">
         <v>273</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="28" t="s">
         <v>269</v>
       </c>
     </row>

</xml_diff>

<commit_message>
WIP voor Blik. Updates op data
</commit_message>
<xml_diff>
--- a/Blik/Interventiebeleid tabak.xlsx
+++ b/Blik/Interventiebeleid tabak.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="255" windowWidth="15180" windowHeight="7290"/>
+    <workbookView xWindow="120" yWindow="315" windowWidth="15180" windowHeight="7230"/>
   </bookViews>
   <sheets>
     <sheet name="Interventieregels" sheetId="1" r:id="rId1"/>
@@ -1994,8 +1994,8 @@
   <dimension ref="A1:V65"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="75" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <pane ySplit="4" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
correct a misplaced commit and move it to "Blik"
</commit_message>
<xml_diff>
--- a/Blik/Interventiebeleid tabak.xlsx
+++ b/Blik/Interventiebeleid tabak.xlsx
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Interventieregels!$C$1:$V$65</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -1006,9 +1006,6 @@
     <t>typeInspecteur</t>
   </si>
   <si>
-    <t>controleItem</t>
-  </si>
-  <si>
     <t>1a</t>
   </si>
   <si>
@@ -1271,6 +1268,9 @@
   </si>
   <si>
     <t>IB02 SPEC 31</t>
+  </si>
+  <si>
+    <t>controleElement</t>
   </si>
 </sst>
 </file>
@@ -1993,9 +1993,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V65"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="75" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="B1" zoomScale="75" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -2024,7 +2024,7 @@
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="47" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E1" s="47"/>
       <c r="F1" s="47"/>
@@ -2136,10 +2136,10 @@
         <v>92</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="3" t="s">
@@ -2170,7 +2170,7 @@
         <v>118</v>
       </c>
       <c r="N4" s="39" t="s">
-        <v>291</v>
+        <v>379</v>
       </c>
       <c r="O4" s="39" t="s">
         <v>290</v>
@@ -2202,10 +2202,10 @@
         <v>93</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="3" t="s">
@@ -2263,13 +2263,13 @@
     </row>
     <row r="6" spans="1:22" s="7" customFormat="1" ht="110.25" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>20</v>
@@ -2310,13 +2310,13 @@
     </row>
     <row r="7" spans="1:22" s="7" customFormat="1" ht="110.25" customHeight="1">
       <c r="A7" s="7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>21</v>
@@ -2361,13 +2361,13 @@
     </row>
     <row r="8" spans="1:22" s="7" customFormat="1" ht="110.25" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>21</v>
@@ -2414,13 +2414,13 @@
     </row>
     <row r="9" spans="1:22" s="10" customFormat="1" ht="74.25" customHeight="1">
       <c r="A9" s="7" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>23</v>
@@ -2472,10 +2472,10 @@
     </row>
     <row r="10" spans="1:22" s="10" customFormat="1" ht="74.25" customHeight="1">
       <c r="A10" s="7" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="7"/>
@@ -2514,10 +2514,10 @@
     </row>
     <row r="11" spans="1:22" s="10" customFormat="1" ht="57" customHeight="1">
       <c r="A11" s="7" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C11" s="1">
         <v>2</v>
@@ -2566,10 +2566,10 @@
     </row>
     <row r="12" spans="1:22" s="10" customFormat="1" ht="55.5" customHeight="1">
       <c r="A12" s="7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C12" s="1">
         <v>3</v>
@@ -2620,10 +2620,10 @@
     </row>
     <row r="13" spans="1:22" s="10" customFormat="1" ht="62.25" customHeight="1">
       <c r="A13" s="7" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C13" s="1">
         <v>4</v>
@@ -2672,10 +2672,10 @@
     </row>
     <row r="14" spans="1:22" s="10" customFormat="1" ht="62.25" customHeight="1">
       <c r="A14" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C14" s="1">
         <v>5</v>
@@ -2722,10 +2722,10 @@
     </row>
     <row r="15" spans="1:22" s="10" customFormat="1" ht="75.75" customHeight="1">
       <c r="A15" s="7" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C15" s="1">
         <v>6</v>
@@ -2774,10 +2774,10 @@
     </row>
     <row r="16" spans="1:22" s="10" customFormat="1" ht="75.75" customHeight="1">
       <c r="A16" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C16" s="1">
         <v>7</v>
@@ -2826,10 +2826,10 @@
     </row>
     <row r="17" spans="1:22" s="10" customFormat="1" ht="73.5" customHeight="1">
       <c r="A17" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C17" s="1">
         <v>8</v>
@@ -2876,10 +2876,10 @@
     </row>
     <row r="18" spans="1:22" s="10" customFormat="1" ht="201" customHeight="1">
       <c r="A18" s="7" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C18" s="1">
         <v>9</v>
@@ -2938,10 +2938,10 @@
     </row>
     <row r="19" spans="1:22" s="10" customFormat="1" ht="201" customHeight="1">
       <c r="A19" s="7" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="7"/>
@@ -2995,10 +2995,10 @@
     </row>
     <row r="20" spans="1:22" s="10" customFormat="1" ht="201" customHeight="1">
       <c r="A20" s="7" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="7"/>
@@ -3041,10 +3041,10 @@
     </row>
     <row r="21" spans="1:22" s="10" customFormat="1" ht="58.5" customHeight="1">
       <c r="A21" s="7" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C21" s="1">
         <v>10</v>
@@ -3105,10 +3105,10 @@
     </row>
     <row r="22" spans="1:22" s="10" customFormat="1" ht="60.75" customHeight="1">
       <c r="A22" s="7" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C22" s="1">
         <v>11</v>
@@ -3167,10 +3167,10 @@
     </row>
     <row r="23" spans="1:22" s="10" customFormat="1" ht="64.5" customHeight="1">
       <c r="A23" s="7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C23" s="1">
         <v>12</v>
@@ -3231,10 +3231,10 @@
     </row>
     <row r="24" spans="1:22" s="10" customFormat="1" ht="66.75" customHeight="1">
       <c r="A24" s="7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C24" s="1">
         <v>13</v>
@@ -3295,10 +3295,10 @@
     </row>
     <row r="25" spans="1:22" s="10" customFormat="1" ht="59.25" customHeight="1">
       <c r="A25" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C25" s="1">
         <v>14</v>
@@ -3359,10 +3359,10 @@
     </row>
     <row r="26" spans="1:22" s="10" customFormat="1" ht="59.25" customHeight="1">
       <c r="A26" s="7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="7"/>
@@ -3409,10 +3409,10 @@
     </row>
     <row r="27" spans="1:22" s="10" customFormat="1" ht="59.25" customHeight="1">
       <c r="A27" s="7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="7"/>
@@ -3467,10 +3467,10 @@
     </row>
     <row r="28" spans="1:22" s="10" customFormat="1" ht="121.5" customHeight="1">
       <c r="A28" s="7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C28" s="1">
         <v>15</v>
@@ -3529,10 +3529,10 @@
     </row>
     <row r="29" spans="1:22" s="10" customFormat="1" ht="66.75" customHeight="1">
       <c r="A29" s="7" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C29" s="1">
         <v>16</v>
@@ -3593,10 +3593,10 @@
     </row>
     <row r="30" spans="1:22" s="10" customFormat="1" ht="78" customHeight="1">
       <c r="A30" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C30" s="1">
         <v>17</v>
@@ -3657,10 +3657,10 @@
     </row>
     <row r="31" spans="1:22" s="10" customFormat="1" ht="78" customHeight="1">
       <c r="A31" s="7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C31" s="1">
         <v>19</v>
@@ -3715,10 +3715,10 @@
     </row>
     <row r="32" spans="1:22" s="10" customFormat="1" ht="78" customHeight="1">
       <c r="A32" s="7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C32" s="1">
         <v>31</v>
@@ -3775,10 +3775,10 @@
     </row>
     <row r="33" spans="1:22" s="10" customFormat="1" ht="78" customHeight="1">
       <c r="A33" s="7" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C33" s="1">
         <v>18</v>
@@ -3835,13 +3835,13 @@
     </row>
     <row r="34" spans="1:22" s="10" customFormat="1" ht="78" customHeight="1">
       <c r="A34" s="7" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D34" s="7"/>
       <c r="E34" s="1" t="s">
@@ -3893,13 +3893,13 @@
     </row>
     <row r="35" spans="1:22" s="10" customFormat="1" ht="78" customHeight="1">
       <c r="A35" s="7" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="1" t="s">
@@ -3951,13 +3951,13 @@
     </row>
     <row r="36" spans="1:22" s="10" customFormat="1" ht="78" customHeight="1">
       <c r="A36" s="7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="1" t="s">
@@ -4009,13 +4009,13 @@
     </row>
     <row r="37" spans="1:22" s="10" customFormat="1" ht="78" customHeight="1">
       <c r="A37" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="1" t="s">
@@ -4065,13 +4065,13 @@
     </row>
     <row r="38" spans="1:22" s="10" customFormat="1" ht="78" customHeight="1">
       <c r="A38" s="7" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D38" s="7"/>
       <c r="E38" s="1" t="s">
@@ -4123,13 +4123,13 @@
     </row>
     <row r="39" spans="1:22" s="10" customFormat="1" ht="78" customHeight="1">
       <c r="A39" s="7" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D39" s="7"/>
       <c r="E39" s="1" t="s">
@@ -4181,13 +4181,13 @@
     </row>
     <row r="40" spans="1:22" s="10" customFormat="1" ht="78" customHeight="1">
       <c r="A40" s="7" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D40" s="7"/>
       <c r="E40" s="1" t="s">
@@ -4237,13 +4237,13 @@
     </row>
     <row r="41" spans="1:22" s="10" customFormat="1" ht="78" customHeight="1">
       <c r="A41" s="7" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D41" s="7"/>
       <c r="E41" s="1" t="s">
@@ -4295,13 +4295,13 @@
     </row>
     <row r="42" spans="1:22" s="10" customFormat="1" ht="78" customHeight="1">
       <c r="A42" s="7" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D42" s="7"/>
       <c r="E42" s="1" t="s">
@@ -4353,13 +4353,13 @@
     </row>
     <row r="43" spans="1:22" s="10" customFormat="1" ht="78" customHeight="1">
       <c r="A43" s="7" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D43" s="7"/>
       <c r="E43" s="1" t="s">
@@ -4413,13 +4413,13 @@
     </row>
     <row r="44" spans="1:22" s="10" customFormat="1" ht="78" customHeight="1">
       <c r="A44" s="7" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D44" s="7"/>
       <c r="E44" s="1" t="s">
@@ -4475,13 +4475,13 @@
     </row>
     <row r="45" spans="1:22" s="10" customFormat="1" ht="78" customHeight="1">
       <c r="A45" s="7" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D45" s="7"/>
       <c r="E45" s="1" t="s">
@@ -4537,13 +4537,13 @@
     </row>
     <row r="46" spans="1:22" s="10" customFormat="1" ht="78" customHeight="1">
       <c r="A46" s="7" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D46" s="7"/>
       <c r="E46" s="1" t="s">
@@ -4593,13 +4593,13 @@
     </row>
     <row r="47" spans="1:22" s="10" customFormat="1" ht="78" customHeight="1">
       <c r="A47" s="7" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D47" s="7"/>
       <c r="E47" s="1" t="s">
@@ -4651,13 +4651,13 @@
     </row>
     <row r="48" spans="1:22" s="10" customFormat="1" ht="78" customHeight="1">
       <c r="A48" s="7" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D48" s="7"/>
       <c r="E48" s="1" t="s">
@@ -4709,13 +4709,13 @@
     </row>
     <row r="49" spans="1:22" s="10" customFormat="1" ht="78" customHeight="1">
       <c r="A49" s="7" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D49" s="7"/>
       <c r="E49" s="1" t="s">
@@ -4765,13 +4765,13 @@
     </row>
     <row r="50" spans="1:22" s="10" customFormat="1" ht="78" customHeight="1">
       <c r="A50" s="7" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D50" s="7"/>
       <c r="E50" s="1" t="s">
@@ -4823,13 +4823,13 @@
     </row>
     <row r="51" spans="1:22" s="10" customFormat="1" ht="78" customHeight="1">
       <c r="A51" s="7" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D51" s="7"/>
       <c r="E51" s="1" t="s">
@@ -4883,10 +4883,10 @@
     </row>
     <row r="52" spans="1:22" s="10" customFormat="1" ht="384.75" customHeight="1">
       <c r="A52" s="7" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C52" s="1">
         <v>20</v>
@@ -4933,10 +4933,10 @@
     </row>
     <row r="53" spans="1:22" s="20" customFormat="1" ht="366" customHeight="1">
       <c r="A53" s="7" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C53" s="17">
         <v>32</v>
@@ -4981,10 +4981,10 @@
     </row>
     <row r="54" spans="1:22" s="10" customFormat="1" ht="346.5" customHeight="1">
       <c r="A54" s="7" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C54" s="1">
         <v>21</v>
@@ -5027,10 +5027,10 @@
     </row>
     <row r="55" spans="1:22" s="10" customFormat="1" ht="354" customHeight="1">
       <c r="A55" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C55" s="1">
         <v>22</v>
@@ -5073,10 +5073,10 @@
     </row>
     <row r="56" spans="1:22" s="20" customFormat="1" ht="354" customHeight="1">
       <c r="A56" s="7" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C56" s="17">
         <v>33</v>
@@ -5119,10 +5119,10 @@
     </row>
     <row r="57" spans="1:22" s="10" customFormat="1" ht="366" customHeight="1">
       <c r="A57" s="10" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C57" s="1">
         <v>23</v>
@@ -5163,10 +5163,10 @@
     </row>
     <row r="58" spans="1:22" s="20" customFormat="1" ht="366" customHeight="1">
       <c r="A58" s="20" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C58" s="17">
         <v>34</v>
@@ -5207,10 +5207,10 @@
     </row>
     <row r="59" spans="1:22" s="10" customFormat="1" ht="354" customHeight="1">
       <c r="A59" s="10" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C59" s="1">
         <v>24</v>
@@ -5251,10 +5251,10 @@
     </row>
     <row r="60" spans="1:22" s="10" customFormat="1" ht="354" customHeight="1">
       <c r="A60" s="10" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C60" s="1">
         <v>25</v>
@@ -5295,10 +5295,10 @@
     </row>
     <row r="61" spans="1:22" s="10" customFormat="1" ht="89.25">
       <c r="A61" s="10" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C61" s="1">
         <v>26</v>
@@ -5347,10 +5347,10 @@
     </row>
     <row r="62" spans="1:22" s="10" customFormat="1" ht="63" customHeight="1">
       <c r="A62" s="10" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C62" s="1">
         <v>27</v>
@@ -5401,10 +5401,10 @@
     </row>
     <row r="63" spans="1:22" s="10" customFormat="1" ht="66.75" customHeight="1">
       <c r="A63" s="10" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C63" s="1">
         <v>28</v>
@@ -5455,10 +5455,10 @@
     </row>
     <row r="64" spans="1:22" s="10" customFormat="1" ht="66.75" customHeight="1">
       <c r="A64" s="10" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C64" s="1">
         <v>29</v>
@@ -5509,10 +5509,10 @@
     </row>
     <row r="65" spans="1:22" s="10" customFormat="1" ht="25.5">
       <c r="A65" s="10" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C65" s="1">
         <v>30</v>

</xml_diff>